<commit_message>
execution of system testing for manager role
</commit_message>
<xml_diff>
--- a/System Testing.xlsx
+++ b/System Testing.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\My-Python-Hub\GithubRepos\Guru99-SW-Tesing-Project-1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1FBE8A5A-2D48-4060-A998-91296390ECC1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E46EFF34-753A-4742-A013-31C902B14966}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-4110" yWindow="-16320" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{6EB662A9-0449-4850-9C79-E79B3BE05DA1}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="348" uniqueCount="235">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="430" uniqueCount="252">
   <si>
     <t>TestCase#</t>
   </si>
@@ -353,13 +353,6 @@
     <t>customer doesn't exist</t>
   </si>
   <si>
-    <t>Verify all accounts of a  deleted Customer are gone</t>
-  </si>
-  <si>
-    <t>check second account is deleted via
- mini statement</t>
-  </si>
-  <si>
     <t xml:space="preserve">Verify Manager can change his Password
 and redirected to the login screen </t>
   </si>
@@ -821,13 +814,75 @@
   </si>
   <si>
     <t>transaction are shown</t>
+  </si>
+  <si>
+    <t>User is not valid</t>
+  </si>
+  <si>
+    <t>Pass</t>
+  </si>
+  <si>
+    <t>Password is Changed
+&amp; redirected to login</t>
+  </si>
+  <si>
+    <t>Sys_M_033</t>
+  </si>
+  <si>
+    <t>Verify New Customer cannot be made with the same records</t>
+  </si>
+  <si>
+    <t>customer cannot be created twice</t>
+  </si>
+  <si>
+    <t>1) Enter same Customer records as previous test case
+2) Submit</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Customer cannot be Created </t>
+  </si>
+  <si>
+    <t>Email Address 
+Already Exist !!</t>
+  </si>
+  <si>
+    <t>HTTP ERROR 500</t>
+  </si>
+  <si>
+    <t>Fail</t>
+  </si>
+  <si>
+    <t>Blank Page</t>
+  </si>
+  <si>
+    <t>Date Error</t>
+  </si>
+  <si>
+    <t>Retest</t>
+  </si>
+  <si>
+    <t>Customer could not be deleted!!. 
+First delete all accounts of this customer then delete the customer</t>
+  </si>
+  <si>
+    <t>You Have Succesfully Logged Out!!</t>
+  </si>
+  <si>
+    <t>Verify customer cannot be deleted if he has accounts</t>
+  </si>
+  <si>
+    <t>check customer is deleted  if he has accounts</t>
+  </si>
+  <si>
+    <t>Password is 
+Changed</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -846,8 +901,29 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C5700"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -860,8 +936,29 @@
         <bgColor rgb="FFD9EAD3"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="4">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -910,11 +1007,27 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -940,8 +1053,23 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="1" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="4">
+    <cellStyle name="Bad" xfId="2" builtinId="27"/>
+    <cellStyle name="Good" xfId="1" builtinId="26"/>
+    <cellStyle name="Neutral" xfId="3" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -955,6 +1083,319 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>361950</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>332838</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>180423</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Picture 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BF4E7355-4542-551C-E139-9DC3DBCA9C73}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="17545050" y="390525"/>
+          <a:ext cx="4295238" cy="4419048"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>390525</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>189984</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>332925</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="5" name="Picture 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A3405DA9-264F-A23C-9413-A6C061A9DF04}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="17573625" y="5867400"/>
+          <a:ext cx="4123809" cy="3600000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>133350</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>570988</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>323401</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="6" name="Picture 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{77E2ED9D-52E8-EF02-463D-7661CBD4E4D8}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="21640800" y="5867400"/>
+          <a:ext cx="4095238" cy="3590476"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>438150</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>370790</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>333094</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="8" name="Picture 7">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0D9ECFE7-D3DA-B853-7E40-FBAE33776F4E}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="19097625" y="9982200"/>
+          <a:ext cx="5476190" cy="2247619"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>495300</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>304800</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>304131</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>161643</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="10" name="Picture 9">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{39A98ED8-07A8-2C07-1F8B-1028C1CDFB83}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="19154775" y="12201525"/>
+          <a:ext cx="5352381" cy="2257143"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>200025</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>314325</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>1571069</xdr:colOff>
+      <xdr:row>46</xdr:row>
+      <xdr:rowOff>151834</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="11" name="Picture 10">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D0927901-9FAE-1A8A-2878-8FAE193299F4}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId6"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5743575" y="16173450"/>
+          <a:ext cx="4447619" cy="4523809"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>1781175</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>1447275</xdr:colOff>
+      <xdr:row>44</xdr:row>
+      <xdr:rowOff>247198</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="12" name="Picture 11">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7C0209F3-48D5-7DF1-FF07-B62A1873FDF5}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId7"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="10401300" y="16392525"/>
+          <a:ext cx="4200000" cy="3619048"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1254,10 +1695,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9E2954B1-BF44-4DD2-B5CD-20514E65DDC8}">
-  <dimension ref="A1:I33"/>
+  <dimension ref="A1:N40"/>
   <sheetViews>
-    <sheetView topLeftCell="A18" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A33"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="30.75" customHeight="1"/>
@@ -1268,12 +1709,15 @@
     <col min="4" max="4" width="46.140625" style="4" customWidth="1"/>
     <col min="5" max="5" width="47.85546875" style="4" customWidth="1"/>
     <col min="6" max="6" width="20.140625" style="4" customWidth="1"/>
-    <col min="7" max="7" width="28.28515625" style="4" customWidth="1"/>
-    <col min="8" max="9" width="16.85546875" style="4" customWidth="1"/>
-    <col min="10" max="16384" width="9.140625" style="4"/>
+    <col min="7" max="7" width="27.85546875" style="4" customWidth="1"/>
+    <col min="8" max="8" width="33" style="4" customWidth="1"/>
+    <col min="9" max="9" width="12.5703125" style="2" customWidth="1"/>
+    <col min="10" max="11" width="9.140625" style="4"/>
+    <col min="12" max="14" width="9.42578125" style="4" customWidth="1"/>
+    <col min="15" max="16384" width="9.140625" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="19.5" customHeight="1">
+    <row r="1" spans="1:14" ht="19.5" customHeight="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1298,16 +1742,16 @@
       <c r="H1" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="I1" s="3" t="s">
+      <c r="I1" s="1" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="30.75" customHeight="1">
+    <row r="2" spans="1:14" ht="30.75" customHeight="1">
       <c r="A2" s="2" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="C2" s="4" t="s">
         <v>27</v>
@@ -1324,10 +1768,16 @@
       <c r="G2" s="4" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="3" spans="1:9" ht="30.75" customHeight="1">
+      <c r="H2" s="4" t="s">
+        <v>233</v>
+      </c>
+      <c r="I2" s="9" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" ht="30.75" customHeight="1">
       <c r="A3" s="2" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="C3" s="4" t="s">
         <v>28</v>
@@ -1344,10 +1794,16 @@
       <c r="G3" s="4" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="4" spans="1:9" ht="30.75" customHeight="1">
+      <c r="H3" s="4" t="s">
+        <v>233</v>
+      </c>
+      <c r="I3" s="9" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" ht="30.75" customHeight="1">
       <c r="A4" s="2" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="C4" s="4" t="s">
         <v>29</v>
@@ -1364,13 +1820,19 @@
       <c r="G4" s="4" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="5" spans="1:9" ht="33" customHeight="1">
+      <c r="H4" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="I4" s="9" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" ht="33" customHeight="1">
       <c r="A5" s="2" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="D5" s="4" t="s">
         <v>10</v>
@@ -1384,10 +1846,16 @@
       <c r="G5" s="5" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="6" spans="1:9" ht="33" customHeight="1">
+      <c r="H5" s="5" t="s">
+        <v>235</v>
+      </c>
+      <c r="I5" s="9" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" ht="33" customHeight="1">
       <c r="A6" s="2" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="C6" s="4" t="s">
         <v>30</v>
@@ -1404,10 +1872,16 @@
       <c r="G6" s="4" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="7" spans="1:9" ht="30.75" customHeight="1">
+      <c r="H6" s="4" t="s">
+        <v>233</v>
+      </c>
+      <c r="I6" s="9" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" ht="30.75" customHeight="1">
       <c r="A7" s="2" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="C7" s="4" t="s">
         <v>31</v>
@@ -1424,10 +1898,16 @@
       <c r="G7" s="4" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="8" spans="1:9" ht="30.75" customHeight="1">
+      <c r="H7" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="I7" s="9" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" ht="30.75" customHeight="1">
       <c r="A8" s="2" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>32</v>
@@ -1447,270 +1927,358 @@
       <c r="G8" s="5" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="9" spans="1:9" ht="47.25" customHeight="1">
+      <c r="H8" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="I8" s="9" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" ht="30.75" customHeight="1">
       <c r="A9" s="2" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="C9" s="5" t="s">
+        <v>237</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>238</v>
+      </c>
+      <c r="E9" s="5" t="s">
+        <v>239</v>
+      </c>
+      <c r="F9" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="G9" s="5" t="s">
+        <v>240</v>
+      </c>
+      <c r="H9" s="5" t="s">
+        <v>241</v>
+      </c>
+      <c r="I9" s="9" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" ht="47.25" customHeight="1">
+      <c r="A10" s="2" t="s">
+        <v>187</v>
+      </c>
+      <c r="C10" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="D9" s="5" t="s">
+      <c r="D10" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="E9" s="5" t="s">
+      <c r="E10" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="F9" s="5" t="s">
+      <c r="F10" s="5" t="s">
         <v>56</v>
-      </c>
-      <c r="G9" s="5" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" ht="47.25" customHeight="1">
-      <c r="A10" s="2" t="s">
-        <v>189</v>
-      </c>
-      <c r="C10" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="D10" s="5" t="s">
-        <v>65</v>
-      </c>
-      <c r="E10" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="F10" s="5" t="s">
-        <v>62</v>
       </c>
       <c r="G10" s="5" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="11" spans="1:9" ht="30.75" customHeight="1">
+      <c r="H10" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="I10" s="9" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" ht="47.25" customHeight="1">
       <c r="A11" s="2" t="s">
+        <v>188</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="D11" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="E11" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="F11" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="G11" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="H11" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="I11" s="9" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" ht="30.75" customHeight="1">
+      <c r="A12" s="2" t="s">
+        <v>189</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="D12" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="E12" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="F12" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="G12" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="H12" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="I12" s="9" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" ht="30.75" customHeight="1">
+      <c r="A13" s="2" t="s">
         <v>190</v>
       </c>
-      <c r="B11" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="C11" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="D11" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="E11" s="5" t="s">
-        <v>52</v>
-      </c>
-      <c r="F11" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="G11" s="5" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" ht="30.75" customHeight="1">
-      <c r="A12" s="2" t="s">
-        <v>191</v>
-      </c>
-      <c r="C12" s="4" t="s">
+      <c r="C13" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="D12" s="4" t="s">
+      <c r="D13" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="E12" s="5" t="s">
+      <c r="E13" s="5" t="s">
         <v>53</v>
-      </c>
-      <c r="F12" s="5" t="s">
-        <v>68</v>
-      </c>
-      <c r="G12" s="5" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" ht="30.75" customHeight="1">
-      <c r="A13" s="2" t="s">
-        <v>192</v>
-      </c>
-      <c r="B13" s="6" t="s">
-        <v>42</v>
-      </c>
-      <c r="C13" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="D13" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="E13" s="5" t="s">
-        <v>66</v>
       </c>
       <c r="F13" s="5" t="s">
         <v>68</v>
       </c>
       <c r="G13" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="H13" s="4" t="s">
+        <v>242</v>
+      </c>
+      <c r="I13" s="11" t="s">
+        <v>243</v>
+      </c>
+      <c r="M13" s="2">
+        <v>31743</v>
+      </c>
+      <c r="N13" s="2">
+        <v>131870</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" ht="30.75" customHeight="1">
+      <c r="A14" s="2" t="s">
+        <v>191</v>
+      </c>
+      <c r="B14" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="D14" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="E14" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="F14" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="G14" s="5" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="14" spans="1:9" ht="30.75" customHeight="1">
-      <c r="A14" s="2" t="s">
+      <c r="H14" s="4" t="s">
+        <v>242</v>
+      </c>
+      <c r="I14" s="11" t="s">
+        <v>243</v>
+      </c>
+      <c r="M14" s="2"/>
+      <c r="N14" s="10">
+        <v>131871</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" ht="30.75" customHeight="1">
+      <c r="A15" s="2" t="s">
+        <v>192</v>
+      </c>
+      <c r="B15" s="6"/>
+      <c r="C15" s="5" t="s">
+        <v>110</v>
+      </c>
+      <c r="D15" s="5" t="s">
+        <v>111</v>
+      </c>
+      <c r="E15" s="5" t="s">
+        <v>112</v>
+      </c>
+      <c r="F15" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="G15" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="H15" s="4" t="s">
+        <v>242</v>
+      </c>
+      <c r="I15" s="11" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" ht="30.75" customHeight="1">
+      <c r="A16" s="2" t="s">
         <v>193</v>
       </c>
-      <c r="B14" s="6"/>
-      <c r="C14" s="5" t="s">
-        <v>112</v>
-      </c>
-      <c r="D14" s="5" t="s">
-        <v>113</v>
-      </c>
-      <c r="E14" s="5" t="s">
-        <v>114</v>
-      </c>
-      <c r="F14" s="5" t="s">
-        <v>74</v>
-      </c>
-      <c r="G14" s="5" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" ht="30.75" customHeight="1">
-      <c r="A15" s="2" t="s">
-        <v>194</v>
-      </c>
-      <c r="C15" s="4" t="s">
+      <c r="C16" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="D15" s="5" t="s">
+      <c r="D16" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="E15" s="5" t="s">
+      <c r="E16" s="5" t="s">
         <v>67</v>
-      </c>
-      <c r="F15" s="5" t="s">
-        <v>68</v>
-      </c>
-      <c r="G15" s="5" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" ht="46.5" customHeight="1">
-      <c r="A16" s="2" t="s">
-        <v>195</v>
-      </c>
-      <c r="C16" s="5" t="s">
-        <v>109</v>
-      </c>
-      <c r="D16" s="5" t="s">
-        <v>110</v>
-      </c>
-      <c r="E16" s="5" t="s">
-        <v>117</v>
       </c>
       <c r="F16" s="5" t="s">
         <v>68</v>
       </c>
       <c r="G16" s="5" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" ht="46.5" customHeight="1">
+        <v>60</v>
+      </c>
+      <c r="H16" s="4" t="s">
+        <v>244</v>
+      </c>
+      <c r="I16" s="11" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" ht="46.5" customHeight="1">
       <c r="A17" s="2" t="s">
+        <v>194</v>
+      </c>
+      <c r="C17" s="5" t="s">
+        <v>107</v>
+      </c>
+      <c r="D17" s="5" t="s">
+        <v>108</v>
+      </c>
+      <c r="E17" s="5" t="s">
+        <v>115</v>
+      </c>
+      <c r="F17" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="G17" s="5" t="s">
+        <v>109</v>
+      </c>
+      <c r="H17" s="5" t="s">
+        <v>109</v>
+      </c>
+      <c r="I17" s="9" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" ht="46.5" customHeight="1">
+      <c r="A18" s="2" t="s">
+        <v>195</v>
+      </c>
+      <c r="B18" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="C18" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="D18" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="E18" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="F18" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="G18" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="H18" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="I18" s="9" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" ht="30.75" customHeight="1">
+      <c r="A19" s="2" t="s">
         <v>196</v>
       </c>
-      <c r="B17" s="6" t="s">
-        <v>61</v>
-      </c>
-      <c r="C17" s="4" t="s">
-        <v>69</v>
-      </c>
-      <c r="D17" s="4" t="s">
-        <v>63</v>
-      </c>
-      <c r="E17" s="5" t="s">
-        <v>70</v>
-      </c>
-      <c r="F17" s="5" t="s">
-        <v>75</v>
-      </c>
-      <c r="G17" s="5" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" ht="30.75" customHeight="1">
-      <c r="A18" s="2" t="s">
-        <v>197</v>
-      </c>
-      <c r="C18" s="4" t="s">
+      <c r="C19" s="4" t="s">
         <v>71</v>
       </c>
-      <c r="D18" s="5" t="s">
+      <c r="D19" s="5" t="s">
         <v>72</v>
       </c>
-      <c r="E18" s="5" t="s">
+      <c r="E19" s="5" t="s">
         <v>73</v>
-      </c>
-      <c r="F18" s="5" t="s">
-        <v>68</v>
-      </c>
-      <c r="G18" s="4" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" ht="46.5" customHeight="1">
-      <c r="A19" s="2" t="s">
-        <v>198</v>
-      </c>
-      <c r="B19" s="6"/>
-      <c r="C19" s="5" t="s">
-        <v>116</v>
-      </c>
-      <c r="D19" s="4" t="s">
-        <v>118</v>
-      </c>
-      <c r="E19" s="5" t="s">
-        <v>119</v>
       </c>
       <c r="F19" s="5" t="s">
         <v>68</v>
       </c>
       <c r="G19" s="4" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" ht="30.75" customHeight="1">
+        <v>124</v>
+      </c>
+      <c r="H19" s="4" t="s">
+        <v>244</v>
+      </c>
+      <c r="I19" s="11" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" ht="46.5" customHeight="1">
       <c r="A20" s="2" t="s">
-        <v>199</v>
-      </c>
-      <c r="B20" s="2" t="s">
-        <v>97</v>
-      </c>
-      <c r="C20" s="4" t="s">
-        <v>76</v>
+        <v>197</v>
+      </c>
+      <c r="B20" s="6"/>
+      <c r="C20" s="5" t="s">
+        <v>114</v>
       </c>
       <c r="D20" s="4" t="s">
-        <v>77</v>
+        <v>116</v>
       </c>
       <c r="E20" s="5" t="s">
-        <v>73</v>
+        <v>117</v>
       </c>
       <c r="F20" s="5" t="s">
         <v>68</v>
       </c>
       <c r="G20" s="4" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" ht="30.75" customHeight="1">
+        <v>245</v>
+      </c>
+      <c r="H20" s="4" t="s">
+        <v>244</v>
+      </c>
+      <c r="I20" s="12" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" ht="30.75" customHeight="1">
       <c r="A21" s="2" t="s">
-        <v>200</v>
-      </c>
-      <c r="C21" s="5" t="s">
-        <v>96</v>
+        <v>198</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="C21" s="4" t="s">
+        <v>76</v>
       </c>
       <c r="D21" s="4" t="s">
-        <v>95</v>
+        <v>77</v>
       </c>
       <c r="E21" s="5" t="s">
         <v>73</v>
@@ -1719,15 +2287,21 @@
         <v>68</v>
       </c>
       <c r="G21" s="4" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" ht="30.75" customHeight="1">
+        <v>79</v>
+      </c>
+      <c r="H21" s="4" t="s">
+        <v>242</v>
+      </c>
+      <c r="I21" s="11" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" ht="30.75" customHeight="1">
       <c r="A22" s="2" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="C22" s="5" t="s">
-        <v>101</v>
+        <v>94</v>
       </c>
       <c r="D22" s="4" t="s">
         <v>93</v>
@@ -1741,16 +2315,22 @@
       <c r="G22" s="4" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="23" spans="1:7" ht="30.75" customHeight="1">
+      <c r="H22" s="4" t="s">
+        <v>242</v>
+      </c>
+      <c r="I22" s="11" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" ht="30.75" customHeight="1">
       <c r="A23" s="2" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="C23" s="5" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="D23" s="4" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="E23" s="5" t="s">
         <v>73</v>
@@ -1761,16 +2341,22 @@
       <c r="G23" s="4" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="24" spans="1:7" ht="30.75" customHeight="1">
+      <c r="H23" s="4" t="s">
+        <v>242</v>
+      </c>
+      <c r="I23" s="11" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" ht="30.75" customHeight="1">
       <c r="A24" s="2" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="C24" s="5" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="D24" s="4" t="s">
-        <v>80</v>
+        <v>92</v>
       </c>
       <c r="E24" s="5" t="s">
         <v>73</v>
@@ -1781,39 +2367,51 @@
       <c r="G24" s="4" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="25" spans="1:7" ht="30.75" customHeight="1">
+      <c r="H24" s="4" t="s">
+        <v>244</v>
+      </c>
+      <c r="I24" s="11" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" ht="30.75" customHeight="1">
       <c r="A25" s="2" t="s">
-        <v>204</v>
-      </c>
-      <c r="B25" s="2" t="s">
-        <v>98</v>
-      </c>
-      <c r="C25" s="4" t="s">
-        <v>82</v>
+        <v>202</v>
+      </c>
+      <c r="C25" s="5" t="s">
+        <v>101</v>
       </c>
       <c r="D25" s="4" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="E25" s="5" t="s">
-        <v>84</v>
+        <v>73</v>
       </c>
       <c r="F25" s="5" t="s">
-        <v>51</v>
+        <v>68</v>
       </c>
       <c r="G25" s="4" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7" ht="30.75" customHeight="1">
+        <v>81</v>
+      </c>
+      <c r="H25" s="4" t="s">
+        <v>244</v>
+      </c>
+      <c r="I25" s="11" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" ht="47.25" customHeight="1">
       <c r="A26" s="2" t="s">
-        <v>205</v>
-      </c>
-      <c r="C26" s="5" t="s">
-        <v>99</v>
+        <v>203</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="C26" s="4" t="s">
+        <v>249</v>
       </c>
       <c r="D26" s="4" t="s">
-        <v>100</v>
+        <v>250</v>
       </c>
       <c r="E26" s="5" t="s">
         <v>84</v>
@@ -1822,41 +2420,53 @@
         <v>51</v>
       </c>
       <c r="G26" s="4" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7" ht="30.75" customHeight="1">
+        <v>85</v>
+      </c>
+      <c r="H26" s="5" t="s">
+        <v>247</v>
+      </c>
+      <c r="I26" s="9" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" ht="47.25" customHeight="1">
       <c r="A27" s="2" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="C27" s="4" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="D27" s="4" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="E27" s="5" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="F27" s="5" t="s">
         <v>51</v>
       </c>
       <c r="G27" s="4" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7" ht="30.75" customHeight="1">
+        <v>85</v>
+      </c>
+      <c r="H27" s="5" t="s">
+        <v>247</v>
+      </c>
+      <c r="I27" s="12" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" ht="47.25" customHeight="1">
       <c r="A28" s="2" t="s">
-        <v>207</v>
-      </c>
-      <c r="C28" s="4" t="s">
-        <v>90</v>
-      </c>
-      <c r="D28" s="5" t="s">
-        <v>91</v>
+        <v>205</v>
+      </c>
+      <c r="C28" s="5" t="s">
+        <v>97</v>
+      </c>
+      <c r="D28" s="4" t="s">
+        <v>98</v>
       </c>
       <c r="E28" s="5" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="F28" s="5" t="s">
         <v>51</v>
@@ -1864,16 +2474,22 @@
       <c r="G28" s="4" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="29" spans="1:7" ht="30.75" customHeight="1">
+      <c r="H28" s="5" t="s">
+        <v>247</v>
+      </c>
+      <c r="I28" s="12" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" ht="47.25" customHeight="1">
       <c r="A29" s="2" t="s">
-        <v>208</v>
-      </c>
-      <c r="C29" s="5" t="s">
-        <v>104</v>
+        <v>206</v>
+      </c>
+      <c r="C29" s="4" t="s">
+        <v>86</v>
       </c>
       <c r="D29" s="4" t="s">
-        <v>108</v>
+        <v>87</v>
       </c>
       <c r="E29" s="5" t="s">
         <v>88</v>
@@ -1884,16 +2500,22 @@
       <c r="G29" s="4" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="30" spans="1:7" ht="30.75" customHeight="1">
+      <c r="H29" s="5" t="s">
+        <v>247</v>
+      </c>
+      <c r="I29" s="12" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" ht="47.25" customHeight="1">
       <c r="A30" s="2" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="C30" s="5" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="D30" s="4" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="E30" s="5" t="s">
         <v>88</v>
@@ -1904,16 +2526,22 @@
       <c r="G30" s="4" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="31" spans="1:7" ht="30.75" customHeight="1">
+      <c r="H30" s="5" t="s">
+        <v>247</v>
+      </c>
+      <c r="I30" s="12" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" ht="47.25" customHeight="1">
       <c r="A31" s="2" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="C31" s="5" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="D31" s="4" t="s">
-        <v>87</v>
+        <v>105</v>
       </c>
       <c r="E31" s="5" t="s">
         <v>88</v>
@@ -1924,54 +2552,122 @@
       <c r="G31" s="4" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="32" spans="1:7" ht="30.75" customHeight="1">
+      <c r="H31" s="5" t="s">
+        <v>247</v>
+      </c>
+      <c r="I31" s="12" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" ht="47.25" customHeight="1">
       <c r="A32" s="2" t="s">
-        <v>211</v>
-      </c>
-      <c r="B32" s="2" t="s">
+        <v>209</v>
+      </c>
+      <c r="C32" s="5" t="s">
+        <v>104</v>
+      </c>
+      <c r="D32" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="E32" s="5" t="s">
+        <v>88</v>
+      </c>
+      <c r="F32" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="G32" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="H32" s="5" t="s">
+        <v>247</v>
+      </c>
+      <c r="I32" s="12" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" ht="30.75" customHeight="1">
+      <c r="A33" s="2" t="s">
+        <v>210</v>
+      </c>
+      <c r="B33" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="C33" s="4" t="s">
+        <v>120</v>
+      </c>
+      <c r="D33" s="4" t="s">
         <v>121</v>
       </c>
-      <c r="C32" s="4" t="s">
+      <c r="E33" s="4" t="s">
         <v>122</v>
       </c>
-      <c r="D32" s="4" t="s">
+      <c r="G33" s="5" t="s">
         <v>123</v>
       </c>
-      <c r="E32" s="4" t="s">
-        <v>124</v>
-      </c>
-      <c r="G32" s="5" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" ht="45" customHeight="1">
-      <c r="A33" s="2" t="s">
-        <v>212</v>
-      </c>
-      <c r="B33" s="6" t="s">
-        <v>149</v>
-      </c>
-      <c r="C33" s="7" t="s">
-        <v>153</v>
-      </c>
-      <c r="D33" s="8"/>
+      <c r="H33" s="4" t="s">
+        <v>248</v>
+      </c>
+      <c r="I33" s="9" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" ht="45" customHeight="1">
+      <c r="A34" s="2" t="s">
+        <v>236</v>
+      </c>
+      <c r="B34" s="6" t="s">
+        <v>147</v>
+      </c>
+      <c r="C34" s="7" t="s">
+        <v>151</v>
+      </c>
+      <c r="D34" s="8"/>
+    </row>
+    <row r="36" spans="1:9" ht="30.75" customHeight="1">
+      <c r="B36" s="2">
+        <v>31743</v>
+      </c>
+      <c r="C36" s="2">
+        <v>131870</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" ht="30.75" customHeight="1">
+      <c r="C37" s="2">
+        <v>131871</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" ht="30.75" customHeight="1">
+      <c r="C38" s="2">
+        <v>131873</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" ht="30.75" customHeight="1">
+      <c r="C39" s="2"/>
+    </row>
+    <row r="40" spans="1:9" ht="30.75" customHeight="1">
+      <c r="B40" s="2">
+        <v>35613</v>
+      </c>
+      <c r="C40" s="2">
+        <v>131872</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="C33:D33"/>
+    <mergeCell ref="C34:D34"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{76EA9C7D-F9B9-4927-9349-23AE4A85C0E3}">
-  <dimension ref="A1:I21"/>
+  <dimension ref="A1:L21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="G16" sqref="G16"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="30.75" customHeight="1"/>
@@ -1987,7 +2683,7 @@
     <col min="10" max="16384" width="9.140625" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="19.5" customHeight="1">
+    <row r="1" spans="1:12" ht="19.5" customHeight="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2016,61 +2712,83 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="44.25" customHeight="1">
+    <row r="2" spans="1:12" ht="44.25" customHeight="1">
       <c r="A2" s="2" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="D2" s="5" t="s">
         <v>8</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="F2" s="5" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="G2" s="4" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="3" spans="1:9" ht="30.75" customHeight="1">
+      <c r="H2" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="I2" s="9" t="s">
+        <v>234</v>
+      </c>
+      <c r="K2" s="2">
+        <v>31743</v>
+      </c>
+      <c r="L2" s="2">
+        <v>131870</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" ht="30.75" customHeight="1">
       <c r="A3" s="2" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="D3" s="4" t="s">
         <v>9</v>
       </c>
       <c r="E3" s="5" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="F3" s="5" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="G3" s="4" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="4" spans="1:9" ht="30.75" customHeight="1">
+      <c r="H3" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="I3" s="9" t="s">
+        <v>234</v>
+      </c>
+      <c r="K3" s="2"/>
+      <c r="L3" s="2">
+        <v>131871</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" ht="30.75" customHeight="1">
       <c r="A4" s="2" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="F4" s="5" t="s">
         <v>18</v>
@@ -2078,13 +2796,23 @@
       <c r="G4" s="4" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="5" spans="1:9" ht="32.25" customHeight="1">
+      <c r="H4" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="I4" s="9" t="s">
+        <v>234</v>
+      </c>
+      <c r="K4" s="2"/>
+      <c r="L4" s="2">
+        <v>131873</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" ht="32.25" customHeight="1">
       <c r="A5" s="2" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="D5" s="4" t="s">
         <v>10</v>
@@ -2098,10 +2826,18 @@
       <c r="G5" s="5" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="6" spans="1:9" ht="32.25" customHeight="1">
+      <c r="H5" s="5" t="s">
+        <v>251</v>
+      </c>
+      <c r="I5" s="9" t="s">
+        <v>234</v>
+      </c>
+      <c r="K5" s="2"/>
+      <c r="L5" s="2"/>
+    </row>
+    <row r="6" spans="1:12" ht="32.25" customHeight="1">
       <c r="A6" s="2" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="C6" s="4" t="s">
         <v>30</v>
@@ -2118,10 +2854,22 @@
       <c r="G6" s="4" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="7" spans="1:9" ht="32.25" customHeight="1">
+      <c r="H6" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="I6" s="9" t="s">
+        <v>234</v>
+      </c>
+      <c r="K6" s="2">
+        <v>35613</v>
+      </c>
+      <c r="L6" s="2">
+        <v>131872</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" ht="32.25" customHeight="1">
       <c r="A7" s="2" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="C7" s="4" t="s">
         <v>31</v>
@@ -2138,19 +2886,25 @@
       <c r="G7" s="4" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="8" spans="1:9" ht="32.25" customHeight="1">
+      <c r="H7" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="I7" s="9" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" ht="32.25" customHeight="1">
       <c r="A8" s="2" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="E8" s="5" t="s">
         <v>73</v>
@@ -2159,170 +2913,170 @@
         <v>68</v>
       </c>
       <c r="G8" s="5" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" ht="32.25" customHeight="1">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" ht="32.25" customHeight="1">
       <c r="A9" s="2" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="B9" s="6"/>
       <c r="C9" s="5" t="s">
+        <v>143</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>144</v>
+      </c>
+      <c r="E9" s="5" t="s">
+        <v>153</v>
+      </c>
+      <c r="F9" s="5" t="s">
+        <v>152</v>
+      </c>
+      <c r="G9" s="5" t="s">
         <v>145</v>
       </c>
-      <c r="D9" s="4" t="s">
-        <v>146</v>
-      </c>
-      <c r="E9" s="5" t="s">
-        <v>155</v>
-      </c>
-      <c r="F9" s="5" t="s">
-        <v>154</v>
-      </c>
-      <c r="G9" s="5" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" ht="32.25" customHeight="1">
+    </row>
+    <row r="10" spans="1:12" ht="32.25" customHeight="1">
       <c r="A10" s="2" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="B10" s="6"/>
       <c r="C10" s="5" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="D10" s="4" t="s">
+        <v>154</v>
+      </c>
+      <c r="E10" s="5" t="s">
+        <v>155</v>
+      </c>
+      <c r="F10" s="5" t="s">
         <v>156</v>
       </c>
-      <c r="E10" s="5" t="s">
+      <c r="G10" s="5" t="s">
         <v>157</v>
       </c>
-      <c r="F10" s="5" t="s">
+    </row>
+    <row r="11" spans="1:12" ht="32.25" customHeight="1">
+      <c r="A11" s="2" t="s">
+        <v>220</v>
+      </c>
+      <c r="B11" s="6" t="s">
         <v>158</v>
-      </c>
-      <c r="G10" s="5" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" ht="32.25" customHeight="1">
-      <c r="A11" s="2" t="s">
-        <v>222</v>
-      </c>
-      <c r="B11" s="6" t="s">
-        <v>160</v>
       </c>
       <c r="C11" s="4" t="s">
         <v>69</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="E11" s="5" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="F11" s="5" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="G11" s="5" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" ht="32.25" customHeight="1">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" ht="32.25" customHeight="1">
       <c r="A12" s="2" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="B12" s="6"/>
       <c r="C12" s="5" t="s">
+        <v>159</v>
+      </c>
+      <c r="D12" s="5" t="s">
+        <v>160</v>
+      </c>
+      <c r="E12" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="F12" s="5" t="s">
+        <v>167</v>
+      </c>
+      <c r="G12" s="5" t="s">
         <v>161</v>
       </c>
-      <c r="D12" s="5" t="s">
-        <v>162</v>
-      </c>
-      <c r="E12" s="5" t="s">
-        <v>164</v>
-      </c>
-      <c r="F12" s="5" t="s">
-        <v>169</v>
-      </c>
-      <c r="G12" s="5" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" ht="32.25" customHeight="1">
+    </row>
+    <row r="13" spans="1:12" ht="32.25" customHeight="1">
       <c r="A13" s="2" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="B13" s="6"/>
       <c r="C13" s="5" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="E13" s="5" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="F13" s="5" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="G13" s="5" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" ht="32.25" customHeight="1">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" ht="32.25" customHeight="1">
       <c r="A14" s="2" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="B14" s="6"/>
       <c r="C14" s="5" t="s">
+        <v>165</v>
+      </c>
+      <c r="D14" s="4" t="s">
+        <v>166</v>
+      </c>
+      <c r="E14" s="5" t="s">
+        <v>170</v>
+      </c>
+      <c r="F14" s="5" t="s">
         <v>167</v>
       </c>
-      <c r="D14" s="4" t="s">
-        <v>168</v>
-      </c>
-      <c r="E14" s="5" t="s">
-        <v>172</v>
-      </c>
-      <c r="F14" s="5" t="s">
-        <v>169</v>
-      </c>
       <c r="G14" s="5" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" ht="32.25" customHeight="1">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" ht="32.25" customHeight="1">
       <c r="A15" s="2" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="B15" s="6"/>
       <c r="C15" s="5" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="D15" s="5" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="E15" s="5" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="F15" s="5" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="G15" s="5" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" ht="32.25" customHeight="1">
+      <c r="A16" s="2" t="s">
+        <v>225</v>
+      </c>
+      <c r="B16" s="6" t="s">
         <v>139</v>
       </c>
-    </row>
-    <row r="16" spans="1:9" ht="32.25" customHeight="1">
-      <c r="A16" s="2" t="s">
-        <v>227</v>
-      </c>
-      <c r="B16" s="6" t="s">
-        <v>141</v>
-      </c>
       <c r="C16" s="4" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="D16" s="4" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="E16" s="5" t="s">
         <v>73</v>
@@ -2331,36 +3085,36 @@
         <v>68</v>
       </c>
       <c r="G16" s="4" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
     </row>
     <row r="17" spans="1:7" ht="32.25" customHeight="1">
       <c r="A17" s="2" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="B17" s="6"/>
       <c r="C17" s="5" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="D17" s="4" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="E17" s="5" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="F17" s="5" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="G17" s="4" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
     </row>
     <row r="18" spans="1:7" ht="30.75" customHeight="1">
       <c r="A18" s="2" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="C18" s="4" t="s">
         <v>71</v>
@@ -2375,69 +3129,69 @@
         <v>68</v>
       </c>
       <c r="G18" s="4" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
     </row>
     <row r="19" spans="1:7" ht="32.25" customHeight="1">
       <c r="A19" s="2" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="B19" s="6"/>
       <c r="C19" s="5" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="D19" s="4" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="E19" s="5" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="F19" s="5" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="G19" s="4" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
     </row>
     <row r="20" spans="1:7" ht="46.5" customHeight="1">
       <c r="A20" s="2" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="B20" s="6"/>
       <c r="C20" s="5" t="s">
+        <v>114</v>
+      </c>
+      <c r="D20" s="4" t="s">
         <v>116</v>
       </c>
-      <c r="D20" s="4" t="s">
-        <v>118</v>
-      </c>
       <c r="E20" s="5" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="F20" s="5" t="s">
         <v>68</v>
       </c>
       <c r="G20" s="4" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
     </row>
     <row r="21" spans="1:7" ht="30.75" customHeight="1">
       <c r="A21" s="2" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="B21" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="C21" s="4" t="s">
+        <v>120</v>
+      </c>
+      <c r="D21" s="4" t="s">
         <v>121</v>
       </c>
-      <c r="C21" s="4" t="s">
+      <c r="E21" s="4" t="s">
         <v>122</v>
       </c>
-      <c r="D21" s="4" t="s">
+      <c r="G21" s="5" t="s">
         <v>123</v>
-      </c>
-      <c r="E21" s="4" t="s">
-        <v>124</v>
-      </c>
-      <c r="G21" s="5" t="s">
-        <v>125</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
System Test Execution for V4 done
</commit_message>
<xml_diff>
--- a/System Testing.xlsx
+++ b/System Testing.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\My-Python-Hub\GithubRepos\Guru99-SW-Tesing-Project-1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E46EFF34-753A-4742-A013-31C902B14966}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3260A2AC-6527-4364-97EB-10AFAC230361}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-4110" yWindow="-16320" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{6EB662A9-0449-4850-9C79-E79B3BE05DA1}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="430" uniqueCount="252">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="606" uniqueCount="278">
   <si>
     <t>TestCase#</t>
   </si>
@@ -184,10 +184,6 @@
     <t>Verify withdrawing money process</t>
   </si>
   <si>
-    <t>Withdraw an amount then check 
-the Balance &amp; the transaction</t>
-  </si>
-  <si>
     <t>1) Enter valid Customer records
 2) Submit</t>
   </si>
@@ -217,10 +213,6 @@
   </si>
   <si>
     <t>1) Enter valid Customer ID
-2) Submit</t>
-  </si>
-  <si>
-    <t>1) Enter valid Account ID
 2) Submit</t>
   </si>
   <si>
@@ -237,19 +229,7 @@
 ,Initial Deposit: 800</t>
   </si>
   <si>
-    <t>Money Withdrawed 
-Successfully, Balance = 700</t>
-  </si>
-  <si>
     <t>Verify adding money process</t>
-  </si>
-  <si>
-    <t>add an amount then check 
-the Balance &amp; the transaction</t>
-  </si>
-  <si>
-    <t>Money Withdrawed 
-Successfully, Balance = 900</t>
   </si>
   <si>
     <t>Fund Transfer, 
@@ -272,14 +252,6 @@
 (Account 2)</t>
   </si>
   <si>
-    <t>1) Withdraw 100 from Account 1
-2) check the Balance From Balance Enquiry</t>
-  </si>
-  <si>
-    <t>1) Deposit 200 to Account 1
-2) check the transactions from Mini Statement</t>
-  </si>
-  <si>
     <t>Account ID: Account 1</t>
   </si>
   <si>
@@ -318,9 +290,6 @@
 Completed successfully</t>
   </si>
   <si>
-    <t>Account deleted successfully</t>
-  </si>
-  <si>
     <t>check account is deleted via mini statement</t>
   </si>
   <si>
@@ -337,9 +306,6 @@
 2) submit</t>
   </si>
   <si>
-    <t>Customer deleted successfully</t>
-  </si>
-  <si>
     <t>Verify all deleted customer details are gone</t>
   </si>
   <si>
@@ -426,13 +392,6 @@
   </si>
   <si>
     <t>withdraw an amount that is more than current deposit</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1) Withdraw 1000 from Account 1
-</t>
-  </si>
-  <si>
-    <t>Cannot withdraw this amount</t>
   </si>
   <si>
     <t>Verify Customized statement is not generated 
@@ -479,12 +438,6 @@
     <t>Verify Customer can't login with wrong ID</t>
   </si>
   <si>
-    <t>Verify Customer can't login with wrong Password</t>
-  </si>
-  <si>
-    <t>Verify Customer can login with correct ID &amp; Password</t>
-  </si>
-  <si>
     <t xml:space="preserve">Verify Customer can change his Password
 and redirected to the login screen </t>
   </si>
@@ -504,10 +457,6 @@
     <t>transaction completed successfully</t>
   </si>
   <si>
-    <t>Verify customer cannot transfer an amount 
-larger than his own deposit</t>
-  </si>
-  <si>
     <t>check Balance of account 1</t>
   </si>
   <si>
@@ -521,9 +470,6 @@
   </si>
   <si>
     <t>Mini Statement</t>
-  </si>
-  <si>
-    <t>Customized Statement</t>
   </si>
   <si>
     <t>Balance Enquiry</t>
@@ -584,9 +530,6 @@
     <t>Balance is not Displayed / Account does not exist</t>
   </si>
   <si>
-    <t>Fund Transfer</t>
-  </si>
-  <si>
     <t>Verify Fund transfer cannot be made 
 by reloading the Fund transfer page</t>
   </si>
@@ -651,9 +594,6 @@
     <t>Verify customer cannot show Mini Statement of another customer's account</t>
   </si>
   <si>
-    <t>Verify customer cannot show Customized Statement of another customer's account</t>
-  </si>
-  <si>
     <t>Sys_M_001</t>
   </si>
   <si>
@@ -839,9 +779,6 @@
 2) Submit</t>
   </si>
   <si>
-    <t xml:space="preserve">Customer cannot be Created </t>
-  </si>
-  <si>
     <t>Email Address 
 Already Exist !!</t>
   </si>
@@ -876,6 +813,164 @@
   <si>
     <t>Password is 
 Changed</t>
+  </si>
+  <si>
+    <t>Customized 
+Statement</t>
+  </si>
+  <si>
+    <t>Login, 
+Password</t>
+  </si>
+  <si>
+    <t>Fund 
+Transfer</t>
+  </si>
+  <si>
+    <t>Verify customer cannot show Customized
+ Statement of another customer's account</t>
+  </si>
+  <si>
+    <t>Verify customer cannot transfer an
+ amount larger than his own deposit</t>
+  </si>
+  <si>
+    <t>Verify Customer can login 
+with correct ID &amp; Password</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Verify ability to transfer 
+Money between accounts </t>
+  </si>
+  <si>
+    <t>Verify Customer can't login 
+with wrong Password</t>
+  </si>
+  <si>
+    <t>Can't make a deleted account
+check Manager Test cases</t>
+  </si>
+  <si>
+    <t>Your Account Balance is low
+ You cant Transfer Balance !!!</t>
+  </si>
+  <si>
+    <t>Verify customer cannot show Mini Statement of a deleted account</t>
+  </si>
+  <si>
+    <t>check Balance of account 4</t>
+  </si>
+  <si>
+    <t>1) insert Account ID of Account 4
+2) submit</t>
+  </si>
+  <si>
+    <t>Sys_C_021</t>
+  </si>
+  <si>
+    <t>Actual Result v3</t>
+  </si>
+  <si>
+    <t>Actual Result v4</t>
+  </si>
+  <si>
+    <t>Actual Result  V3</t>
+  </si>
+  <si>
+    <t>Actual Result V4</t>
+  </si>
+  <si>
+    <t>Account deleted 
+successfully</t>
+  </si>
+  <si>
+    <t>Customer deleted 
+successfully</t>
+  </si>
+  <si>
+    <t>Cannot withdraw 
+this amount</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Customer cannot 
+be Created </t>
+  </si>
+  <si>
+    <t>Money Withdrawed 
+Successfully</t>
+  </si>
+  <si>
+    <t xml:space="preserve">check the Balance </t>
+  </si>
+  <si>
+    <t>Balance Displayed</t>
+  </si>
+  <si>
+    <t>HTTP ERROR 50</t>
+  </si>
+  <si>
+    <t>check the transactions via  Mini Statement</t>
+  </si>
+  <si>
+    <t xml:space="preserve">withdraw an amount to an account </t>
+  </si>
+  <si>
+    <t>add an amount to an account via deposit</t>
+  </si>
+  <si>
+    <t>1) Enter Account ID
+2) Submit</t>
+  </si>
+  <si>
+    <t>1) Enter Account ID, Amount = 100
+2) Submit</t>
+  </si>
+  <si>
+    <t>Verify Mini Statement</t>
+  </si>
+  <si>
+    <t>Money added 
+Successfully, Balance = 900</t>
+  </si>
+  <si>
+    <t>Transactions Displayed</t>
+  </si>
+  <si>
+    <t>Sys_M_034</t>
+  </si>
+  <si>
+    <t>Sys_M_035</t>
+  </si>
+  <si>
+    <t>Customer 1
+31743</t>
+  </si>
+  <si>
+    <t>Account1:
+131870</t>
+  </si>
+  <si>
+    <t>Account2:
+131871</t>
+  </si>
+  <si>
+    <t>Account3:131873</t>
+  </si>
+  <si>
+    <t>Customer2
+35613</t>
+  </si>
+  <si>
+    <t>Account4
+131872</t>
+  </si>
+  <si>
+    <t>Field changed to dropdown
+Test case Unvalid</t>
+  </si>
+  <si>
+    <t>Payers account No and Payees
+ account No Must Not be Same!!!</t>
   </si>
 </sst>
 </file>
@@ -923,7 +1018,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -951,14 +1046,8 @@
         <fgColor rgb="FFFFEB9C"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFFF"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="5">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -1007,19 +1096,6 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -1027,7 +1103,7 @@
     <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1047,16 +1123,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="2" applyBorder="1" applyAlignment="1">
@@ -1064,6 +1131,12 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="5" borderId="1" xfId="3" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -1089,23 +1162,23 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>361950</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>142875</xdr:rowOff>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>1885950</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>332838</xdr:colOff>
-      <xdr:row>11</xdr:row>
-      <xdr:rowOff>180423</xdr:rowOff>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>3171269</xdr:colOff>
+      <xdr:row>47</xdr:row>
+      <xdr:rowOff>256609</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="4" name="Picture 3">
+        <xdr:cNvPr id="11" name="Picture 10">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BF4E7355-4542-551C-E139-9DC3DBCA9C73}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D0927901-9FAE-1A8A-2878-8FAE193299F4}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1121,8 +1194,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="17545050" y="390525"/>
-          <a:ext cx="4295238" cy="4419048"/>
+          <a:off x="4267200" y="16668750"/>
+          <a:ext cx="4447619" cy="4523809"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1133,23 +1206,23 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>390525</xdr:colOff>
-      <xdr:row>14</xdr:row>
-      <xdr:rowOff>66675</xdr:rowOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>2000250</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>189984</xdr:colOff>
-      <xdr:row>21</xdr:row>
-      <xdr:rowOff>332925</xdr:rowOff>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>75675</xdr:colOff>
+      <xdr:row>45</xdr:row>
+      <xdr:rowOff>132898</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="5" name="Picture 4">
+        <xdr:cNvPr id="12" name="Picture 11">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A3405DA9-264F-A23C-9413-A6C061A9DF04}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7C0209F3-48D5-7DF1-FF07-B62A1873FDF5}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1165,8 +1238,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="17573625" y="5867400"/>
-          <a:ext cx="4123809" cy="3600000"/>
+          <a:off x="16887825" y="16668750"/>
+          <a:ext cx="4200000" cy="3619048"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1177,23 +1250,23 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>133350</xdr:colOff>
-      <xdr:row>14</xdr:row>
-      <xdr:rowOff>66675</xdr:rowOff>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>22</xdr:col>
-      <xdr:colOff>570988</xdr:colOff>
-      <xdr:row>21</xdr:row>
-      <xdr:rowOff>323401</xdr:rowOff>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>1913988</xdr:colOff>
+      <xdr:row>47</xdr:row>
+      <xdr:rowOff>199473</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="6" name="Picture 5">
+        <xdr:cNvPr id="2" name="Picture 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{77E2ED9D-52E8-EF02-463D-7661CBD4E4D8}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6816E130-3D7B-40A9-99FD-69491D2B5E8B}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1209,8 +1282,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="21640800" y="5867400"/>
-          <a:ext cx="4095238" cy="3590476"/>
+          <a:off x="0" y="16716375"/>
+          <a:ext cx="4295238" cy="4419048"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1221,23 +1294,23 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>438150</xdr:colOff>
-      <xdr:row>23</xdr:row>
-      <xdr:rowOff>66675</xdr:rowOff>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>3181350</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>19</xdr:col>
-      <xdr:colOff>370790</xdr:colOff>
-      <xdr:row>27</xdr:row>
-      <xdr:rowOff>333094</xdr:rowOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>923409</xdr:colOff>
+      <xdr:row>45</xdr:row>
+      <xdr:rowOff>113850</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="8" name="Picture 7">
+        <xdr:cNvPr id="3" name="Picture 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0D9ECFE7-D3DA-B853-7E40-FBAE33776F4E}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7F7DF9C1-EC46-4AAF-A99D-D4D8FE49B6A2}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1253,8 +1326,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="19097625" y="9982200"/>
-          <a:ext cx="5476190" cy="2247619"/>
+          <a:off x="8724900" y="16668750"/>
+          <a:ext cx="4123809" cy="3600000"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1265,23 +1338,23 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>495300</xdr:colOff>
-      <xdr:row>28</xdr:row>
-      <xdr:rowOff>304800</xdr:rowOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>657225</xdr:colOff>
+      <xdr:row>45</xdr:row>
+      <xdr:rowOff>361950</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>19</xdr:col>
-      <xdr:colOff>304131</xdr:colOff>
-      <xdr:row>32</xdr:row>
-      <xdr:rowOff>161643</xdr:rowOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>361617</xdr:colOff>
+      <xdr:row>50</xdr:row>
+      <xdr:rowOff>323611</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="10" name="Picture 9">
+        <xdr:cNvPr id="9" name="Picture 8">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{39A98ED8-07A8-2C07-1F8B-1028C1CDFB83}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{14B6C1B7-8B47-E995-DF82-72442DC93DAD}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1297,8 +1370,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="19154775" y="12201525"/>
-          <a:ext cx="5352381" cy="2257143"/>
+          <a:off x="12582525" y="20516850"/>
+          <a:ext cx="2666667" cy="1914286"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1309,23 +1382,23 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>200025</xdr:colOff>
-      <xdr:row>34</xdr:row>
-      <xdr:rowOff>314325</xdr:rowOff>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>790575</xdr:colOff>
+      <xdr:row>45</xdr:row>
+      <xdr:rowOff>371475</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>1571069</xdr:colOff>
-      <xdr:row>46</xdr:row>
-      <xdr:rowOff>151834</xdr:rowOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>218748</xdr:colOff>
+      <xdr:row>50</xdr:row>
+      <xdr:rowOff>342660</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="11" name="Picture 10">
+        <xdr:cNvPr id="13" name="Picture 12">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D0927901-9FAE-1A8A-2878-8FAE193299F4}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0C8122F0-C892-7AF5-0CB3-D4BE18E1608B}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1341,8 +1414,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="5743575" y="16173450"/>
-          <a:ext cx="4447619" cy="4523809"/>
+          <a:off x="9525000" y="20526375"/>
+          <a:ext cx="2619048" cy="1923810"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1353,23 +1426,23 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>1781175</xdr:colOff>
-      <xdr:row>35</xdr:row>
-      <xdr:rowOff>142875</xdr:rowOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>866775</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>1447275</xdr:colOff>
-      <xdr:row>44</xdr:row>
-      <xdr:rowOff>247198</xdr:rowOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>1999738</xdr:colOff>
+      <xdr:row>45</xdr:row>
+      <xdr:rowOff>94801</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="12" name="Picture 11">
+        <xdr:cNvPr id="14" name="Picture 13">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7C0209F3-48D5-7DF1-FF07-B62A1873FDF5}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{276B3490-E816-46E7-9398-21840861B027}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1385,8 +1458,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="10401300" y="16392525"/>
-          <a:ext cx="4200000" cy="3619048"/>
+          <a:off x="12792075" y="16659225"/>
+          <a:ext cx="4095238" cy="3590476"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1695,10 +1768,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9E2954B1-BF44-4DD2-B5CD-20514E65DDC8}">
-  <dimension ref="A1:N40"/>
+  <dimension ref="A1:N36"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I2" sqref="I2"/>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="M13" sqref="M13:N17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="30.75" customHeight="1"/>
@@ -1706,14 +1779,16 @@
     <col min="1" max="1" width="10.140625" style="2" customWidth="1"/>
     <col min="2" max="2" width="25.5703125" style="2" customWidth="1"/>
     <col min="3" max="3" width="47.42578125" style="4" customWidth="1"/>
-    <col min="4" max="4" width="46.140625" style="4" customWidth="1"/>
-    <col min="5" max="5" width="47.85546875" style="4" customWidth="1"/>
+    <col min="4" max="5" width="47.85546875" style="4" customWidth="1"/>
     <col min="6" max="6" width="20.140625" style="4" customWidth="1"/>
-    <col min="7" max="7" width="27.85546875" style="4" customWidth="1"/>
-    <col min="8" max="8" width="33" style="4" customWidth="1"/>
-    <col min="9" max="9" width="12.5703125" style="2" customWidth="1"/>
-    <col min="10" max="11" width="9.140625" style="4"/>
-    <col min="12" max="14" width="9.42578125" style="4" customWidth="1"/>
+    <col min="7" max="7" width="24.28515625" style="4" customWidth="1"/>
+    <col min="8" max="8" width="32.140625" style="4" customWidth="1"/>
+    <col min="9" max="9" width="9" style="2" customWidth="1"/>
+    <col min="10" max="10" width="32.140625" style="4" customWidth="1"/>
+    <col min="11" max="11" width="9.140625" style="4"/>
+    <col min="12" max="12" width="9.42578125" style="4" customWidth="1"/>
+    <col min="13" max="13" width="11.85546875" style="4" customWidth="1"/>
+    <col min="14" max="14" width="9.42578125" style="4" customWidth="1"/>
     <col min="15" max="16384" width="9.140625" style="4"/>
   </cols>
   <sheetData>
@@ -1740,18 +1815,24 @@
         <v>6</v>
       </c>
       <c r="H1" s="3" t="s">
-        <v>14</v>
+        <v>250</v>
       </c>
       <c r="I1" s="1" t="s">
         <v>13</v>
       </c>
+      <c r="J1" s="3" t="s">
+        <v>251</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="2" spans="1:14" ht="30.75" customHeight="1">
       <c r="A2" s="2" t="s">
-        <v>179</v>
+        <v>162</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>118</v>
+        <v>107</v>
       </c>
       <c r="C2" s="4" t="s">
         <v>27</v>
@@ -1769,15 +1850,21 @@
         <v>24</v>
       </c>
       <c r="H2" s="4" t="s">
-        <v>233</v>
-      </c>
-      <c r="I2" s="9" t="s">
-        <v>234</v>
+        <v>216</v>
+      </c>
+      <c r="I2" s="7" t="s">
+        <v>217</v>
+      </c>
+      <c r="J2" s="4" t="s">
+        <v>216</v>
+      </c>
+      <c r="K2" s="7" t="s">
+        <v>217</v>
       </c>
     </row>
     <row r="3" spans="1:14" ht="30.75" customHeight="1">
       <c r="A3" s="2" t="s">
-        <v>180</v>
+        <v>163</v>
       </c>
       <c r="C3" s="4" t="s">
         <v>28</v>
@@ -1795,15 +1882,21 @@
         <v>24</v>
       </c>
       <c r="H3" s="4" t="s">
-        <v>233</v>
-      </c>
-      <c r="I3" s="9" t="s">
-        <v>234</v>
+        <v>216</v>
+      </c>
+      <c r="I3" s="7" t="s">
+        <v>217</v>
+      </c>
+      <c r="J3" s="4" t="s">
+        <v>216</v>
+      </c>
+      <c r="K3" s="7" t="s">
+        <v>217</v>
       </c>
     </row>
     <row r="4" spans="1:14" ht="30.75" customHeight="1">
       <c r="A4" s="2" t="s">
-        <v>181</v>
+        <v>164</v>
       </c>
       <c r="C4" s="4" t="s">
         <v>29</v>
@@ -1823,16 +1916,22 @@
       <c r="H4" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="I4" s="9" t="s">
-        <v>234</v>
+      <c r="I4" s="7" t="s">
+        <v>217</v>
+      </c>
+      <c r="J4" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="K4" s="7" t="s">
+        <v>217</v>
       </c>
     </row>
     <row r="5" spans="1:14" ht="33" customHeight="1">
       <c r="A5" s="2" t="s">
-        <v>182</v>
+        <v>165</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>90</v>
+        <v>81</v>
       </c>
       <c r="D5" s="4" t="s">
         <v>10</v>
@@ -1847,15 +1946,21 @@
         <v>26</v>
       </c>
       <c r="H5" s="5" t="s">
-        <v>235</v>
-      </c>
-      <c r="I5" s="9" t="s">
-        <v>234</v>
+        <v>218</v>
+      </c>
+      <c r="I5" s="7" t="s">
+        <v>217</v>
+      </c>
+      <c r="J5" s="5" t="s">
+        <v>218</v>
+      </c>
+      <c r="K5" s="7" t="s">
+        <v>217</v>
       </c>
     </row>
     <row r="6" spans="1:14" ht="33" customHeight="1">
       <c r="A6" s="2" t="s">
-        <v>183</v>
+        <v>166</v>
       </c>
       <c r="C6" s="4" t="s">
         <v>30</v>
@@ -1873,15 +1978,21 @@
         <v>24</v>
       </c>
       <c r="H6" s="4" t="s">
-        <v>233</v>
-      </c>
-      <c r="I6" s="9" t="s">
-        <v>234</v>
+        <v>216</v>
+      </c>
+      <c r="I6" s="7" t="s">
+        <v>217</v>
+      </c>
+      <c r="J6" s="4" t="s">
+        <v>216</v>
+      </c>
+      <c r="K6" s="7" t="s">
+        <v>217</v>
       </c>
     </row>
     <row r="7" spans="1:14" ht="30.75" customHeight="1">
       <c r="A7" s="2" t="s">
-        <v>184</v>
+        <v>167</v>
       </c>
       <c r="C7" s="4" t="s">
         <v>31</v>
@@ -1901,13 +2012,19 @@
       <c r="H7" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="I7" s="9" t="s">
-        <v>234</v>
+      <c r="I7" s="7" t="s">
+        <v>217</v>
+      </c>
+      <c r="J7" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="K7" s="7" t="s">
+        <v>217</v>
       </c>
     </row>
     <row r="8" spans="1:14" ht="30.75" customHeight="1">
       <c r="A8" s="2" t="s">
-        <v>185</v>
+        <v>168</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>32</v>
@@ -1919,102 +2036,126 @@
         <v>35</v>
       </c>
       <c r="E8" s="5" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F8" s="5" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="G8" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="H8" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="I8" s="9" t="s">
-        <v>234</v>
+        <v>47</v>
+      </c>
+      <c r="I8" s="7" t="s">
+        <v>217</v>
+      </c>
+      <c r="J8" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="K8" s="7" t="s">
+        <v>217</v>
       </c>
     </row>
     <row r="9" spans="1:14" ht="30.75" customHeight="1">
       <c r="A9" s="2" t="s">
-        <v>186</v>
+        <v>169</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>237</v>
+        <v>220</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>238</v>
+        <v>221</v>
       </c>
       <c r="E9" s="5" t="s">
-        <v>239</v>
+        <v>222</v>
       </c>
       <c r="F9" s="5" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="G9" s="5" t="s">
-        <v>240</v>
+        <v>255</v>
       </c>
       <c r="H9" s="5" t="s">
-        <v>241</v>
-      </c>
-      <c r="I9" s="9" t="s">
-        <v>234</v>
+        <v>223</v>
+      </c>
+      <c r="I9" s="7" t="s">
+        <v>217</v>
+      </c>
+      <c r="J9" s="5" t="s">
+        <v>223</v>
+      </c>
+      <c r="K9" s="7" t="s">
+        <v>217</v>
       </c>
     </row>
     <row r="10" spans="1:14" ht="47.25" customHeight="1">
       <c r="A10" s="2" t="s">
-        <v>187</v>
+        <v>170</v>
       </c>
       <c r="C10" s="5" t="s">
         <v>34</v>
       </c>
       <c r="D10" s="5" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="E10" s="5" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="F10" s="5" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="G10" s="5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="H10" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="I10" s="9" t="s">
-        <v>234</v>
+        <v>48</v>
+      </c>
+      <c r="I10" s="7" t="s">
+        <v>217</v>
+      </c>
+      <c r="J10" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="K10" s="7" t="s">
+        <v>217</v>
       </c>
     </row>
     <row r="11" spans="1:14" ht="47.25" customHeight="1">
       <c r="A11" s="2" t="s">
-        <v>188</v>
+        <v>171</v>
       </c>
       <c r="C11" s="4" t="s">
         <v>37</v>
       </c>
       <c r="D11" s="5" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="E11" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F11" s="5" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="G11" s="5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="H11" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="I11" s="9" t="s">
-        <v>234</v>
+        <v>48</v>
+      </c>
+      <c r="I11" s="7" t="s">
+        <v>217</v>
+      </c>
+      <c r="J11" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="K11" s="7" t="s">
+        <v>217</v>
       </c>
     </row>
     <row r="12" spans="1:14" ht="30.75" customHeight="1">
       <c r="A12" s="2" t="s">
-        <v>189</v>
+        <v>172</v>
       </c>
       <c r="B12" s="2" t="s">
         <v>36</v>
@@ -2026,24 +2167,30 @@
         <v>38</v>
       </c>
       <c r="E12" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="F12" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="G12" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="F12" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="G12" s="5" t="s">
-        <v>54</v>
-      </c>
       <c r="H12" s="5" t="s">
-        <v>54</v>
-      </c>
-      <c r="I12" s="9" t="s">
-        <v>234</v>
+        <v>52</v>
+      </c>
+      <c r="I12" s="7" t="s">
+        <v>217</v>
+      </c>
+      <c r="J12" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="K12" s="7" t="s">
+        <v>217</v>
       </c>
     </row>
     <row r="13" spans="1:14" ht="30.75" customHeight="1">
       <c r="A13" s="2" t="s">
-        <v>190</v>
+        <v>173</v>
       </c>
       <c r="C13" s="4" t="s">
         <v>41</v>
@@ -2052,30 +2199,36 @@
         <v>39</v>
       </c>
       <c r="E13" s="5" t="s">
+        <v>263</v>
+      </c>
+      <c r="F13" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="G13" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="F13" s="5" t="s">
-        <v>68</v>
-      </c>
-      <c r="G13" s="5" t="s">
-        <v>55</v>
-      </c>
       <c r="H13" s="4" t="s">
-        <v>242</v>
-      </c>
-      <c r="I13" s="11" t="s">
-        <v>243</v>
-      </c>
-      <c r="M13" s="2">
-        <v>31743</v>
-      </c>
-      <c r="N13" s="2">
-        <v>131870</v>
+        <v>224</v>
+      </c>
+      <c r="I13" s="8" t="s">
+        <v>225</v>
+      </c>
+      <c r="J13" s="4" t="s">
+        <v>224</v>
+      </c>
+      <c r="K13" s="8" t="s">
+        <v>225</v>
+      </c>
+      <c r="M13" s="6" t="s">
+        <v>270</v>
+      </c>
+      <c r="N13" s="6" t="s">
+        <v>271</v>
       </c>
     </row>
     <row r="14" spans="1:14" ht="30.75" customHeight="1">
       <c r="A14" s="2" t="s">
-        <v>191</v>
+        <v>174</v>
       </c>
       <c r="B14" s="6" t="s">
         <v>42</v>
@@ -2084,577 +2237,745 @@
         <v>43</v>
       </c>
       <c r="D14" s="5" t="s">
-        <v>44</v>
+        <v>261</v>
       </c>
       <c r="E14" s="5" t="s">
-        <v>66</v>
+        <v>264</v>
       </c>
       <c r="F14" s="5" t="s">
-        <v>68</v>
+        <v>61</v>
       </c>
       <c r="G14" s="5" t="s">
-        <v>57</v>
+        <v>256</v>
       </c>
       <c r="H14" s="4" t="s">
-        <v>242</v>
-      </c>
-      <c r="I14" s="11" t="s">
-        <v>243</v>
+        <v>224</v>
+      </c>
+      <c r="I14" s="8" t="s">
+        <v>225</v>
+      </c>
+      <c r="J14" s="5" t="s">
+        <v>256</v>
+      </c>
+      <c r="K14" s="7" t="s">
+        <v>217</v>
       </c>
       <c r="M14" s="2"/>
-      <c r="N14" s="10">
-        <v>131871</v>
+      <c r="N14" s="6" t="s">
+        <v>272</v>
       </c>
     </row>
     <row r="15" spans="1:14" ht="30.75" customHeight="1">
       <c r="A15" s="2" t="s">
-        <v>192</v>
+        <v>175</v>
       </c>
       <c r="B15" s="6"/>
-      <c r="C15" s="5" t="s">
-        <v>110</v>
+      <c r="C15" s="4" t="s">
+        <v>127</v>
       </c>
       <c r="D15" s="5" t="s">
-        <v>111</v>
+        <v>257</v>
       </c>
       <c r="E15" s="5" t="s">
-        <v>112</v>
+        <v>263</v>
       </c>
       <c r="F15" s="5" t="s">
-        <v>74</v>
+        <v>67</v>
       </c>
       <c r="G15" s="5" t="s">
-        <v>113</v>
+        <v>258</v>
       </c>
       <c r="H15" s="4" t="s">
-        <v>242</v>
-      </c>
-      <c r="I15" s="11" t="s">
-        <v>243</v>
+        <v>259</v>
+      </c>
+      <c r="I15" s="8" t="s">
+        <v>225</v>
+      </c>
+      <c r="J15" s="4" t="s">
+        <v>224</v>
+      </c>
+      <c r="K15" s="8" t="s">
+        <v>225</v>
+      </c>
+      <c r="M15" s="2"/>
+      <c r="N15" s="6" t="s">
+        <v>273</v>
       </c>
     </row>
     <row r="16" spans="1:14" ht="30.75" customHeight="1">
       <c r="A16" s="2" t="s">
-        <v>193</v>
-      </c>
-      <c r="C16" s="4" t="s">
+        <v>176</v>
+      </c>
+      <c r="B16" s="6"/>
+      <c r="C16" s="5" t="s">
+        <v>101</v>
+      </c>
+      <c r="D16" s="5" t="s">
+        <v>102</v>
+      </c>
+      <c r="E16" s="5" t="s">
+        <v>264</v>
+      </c>
+      <c r="F16" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="G16" s="5" t="s">
+        <v>254</v>
+      </c>
+      <c r="H16" s="4" t="s">
+        <v>224</v>
+      </c>
+      <c r="I16" s="8" t="s">
+        <v>225</v>
+      </c>
+      <c r="J16" s="5" t="s">
+        <v>254</v>
+      </c>
+      <c r="K16" s="7" t="s">
+        <v>217</v>
+      </c>
+      <c r="M16" s="2"/>
+      <c r="N16" s="2"/>
+    </row>
+    <row r="17" spans="1:14" ht="30.75" customHeight="1">
+      <c r="A17" s="2" t="s">
+        <v>177</v>
+      </c>
+      <c r="C17" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="D17" s="5" t="s">
+        <v>262</v>
+      </c>
+      <c r="E17" s="5" t="s">
+        <v>264</v>
+      </c>
+      <c r="F17" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="G17" s="5" t="s">
+        <v>266</v>
+      </c>
+      <c r="H17" s="4" t="s">
+        <v>226</v>
+      </c>
+      <c r="I17" s="8" t="s">
+        <v>225</v>
+      </c>
+      <c r="J17" s="4" t="s">
+        <v>224</v>
+      </c>
+      <c r="K17" s="8" t="s">
+        <v>225</v>
+      </c>
+      <c r="M17" s="6" t="s">
+        <v>274</v>
+      </c>
+      <c r="N17" s="6" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14" ht="30.75" customHeight="1">
+      <c r="A18" s="2" t="s">
+        <v>178</v>
+      </c>
+      <c r="C18" s="4" t="s">
+        <v>265</v>
+      </c>
+      <c r="D18" s="5" t="s">
+        <v>260</v>
+      </c>
+      <c r="E18" s="5" t="s">
+        <v>263</v>
+      </c>
+      <c r="F18" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="G18" s="5" t="s">
+        <v>267</v>
+      </c>
+      <c r="H18" s="4" t="s">
+        <v>226</v>
+      </c>
+      <c r="I18" s="8" t="s">
+        <v>225</v>
+      </c>
+      <c r="J18" s="4" t="s">
+        <v>226</v>
+      </c>
+      <c r="K18" s="8" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="19" spans="1:14" ht="46.5" customHeight="1">
+      <c r="A19" s="2" t="s">
+        <v>179</v>
+      </c>
+      <c r="C19" s="5" t="s">
+        <v>98</v>
+      </c>
+      <c r="D19" s="5" t="s">
+        <v>99</v>
+      </c>
+      <c r="E19" s="5" t="s">
+        <v>104</v>
+      </c>
+      <c r="F19" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="G19" s="5" t="s">
+        <v>100</v>
+      </c>
+      <c r="H19" s="5" t="s">
+        <v>100</v>
+      </c>
+      <c r="I19" s="7" t="s">
+        <v>217</v>
+      </c>
+      <c r="J19" s="5" t="s">
+        <v>100</v>
+      </c>
+      <c r="K19" s="7" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="20" spans="1:14" ht="46.5" customHeight="1">
+      <c r="A20" s="2" t="s">
+        <v>180</v>
+      </c>
+      <c r="B20" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="C20" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="D20" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="D16" s="5" t="s">
-        <v>59</v>
-      </c>
-      <c r="E16" s="5" t="s">
-        <v>67</v>
-      </c>
-      <c r="F16" s="5" t="s">
-        <v>68</v>
-      </c>
-      <c r="G16" s="5" t="s">
-        <v>60</v>
-      </c>
-      <c r="H16" s="4" t="s">
-        <v>244</v>
-      </c>
-      <c r="I16" s="11" t="s">
-        <v>243</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9" ht="46.5" customHeight="1">
-      <c r="A17" s="2" t="s">
-        <v>194</v>
-      </c>
-      <c r="C17" s="5" t="s">
-        <v>107</v>
-      </c>
-      <c r="D17" s="5" t="s">
-        <v>108</v>
-      </c>
-      <c r="E17" s="5" t="s">
-        <v>115</v>
-      </c>
-      <c r="F17" s="5" t="s">
-        <v>68</v>
-      </c>
-      <c r="G17" s="5" t="s">
-        <v>109</v>
-      </c>
-      <c r="H17" s="5" t="s">
-        <v>109</v>
-      </c>
-      <c r="I17" s="9" t="s">
-        <v>234</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9" ht="46.5" customHeight="1">
-      <c r="A18" s="2" t="s">
-        <v>195</v>
-      </c>
-      <c r="B18" s="6" t="s">
-        <v>61</v>
-      </c>
-      <c r="C18" s="4" t="s">
-        <v>69</v>
-      </c>
-      <c r="D18" s="4" t="s">
+      <c r="E20" s="5" t="s">
         <v>63</v>
-      </c>
-      <c r="E18" s="5" t="s">
-        <v>70</v>
-      </c>
-      <c r="F18" s="5" t="s">
-        <v>75</v>
-      </c>
-      <c r="G18" s="5" t="s">
-        <v>78</v>
-      </c>
-      <c r="H18" s="5" t="s">
-        <v>78</v>
-      </c>
-      <c r="I18" s="9" t="s">
-        <v>234</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9" ht="30.75" customHeight="1">
-      <c r="A19" s="2" t="s">
-        <v>196</v>
-      </c>
-      <c r="C19" s="4" t="s">
-        <v>71</v>
-      </c>
-      <c r="D19" s="5" t="s">
-        <v>72</v>
-      </c>
-      <c r="E19" s="5" t="s">
-        <v>73</v>
-      </c>
-      <c r="F19" s="5" t="s">
-        <v>68</v>
-      </c>
-      <c r="G19" s="4" t="s">
-        <v>124</v>
-      </c>
-      <c r="H19" s="4" t="s">
-        <v>244</v>
-      </c>
-      <c r="I19" s="11" t="s">
-        <v>243</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9" ht="46.5" customHeight="1">
-      <c r="A20" s="2" t="s">
-        <v>197</v>
-      </c>
-      <c r="B20" s="6"/>
-      <c r="C20" s="5" t="s">
-        <v>114</v>
-      </c>
-      <c r="D20" s="4" t="s">
-        <v>116</v>
-      </c>
-      <c r="E20" s="5" t="s">
-        <v>117</v>
       </c>
       <c r="F20" s="5" t="s">
         <v>68</v>
       </c>
-      <c r="G20" s="4" t="s">
-        <v>245</v>
-      </c>
-      <c r="H20" s="4" t="s">
-        <v>244</v>
-      </c>
-      <c r="I20" s="12" t="s">
-        <v>246</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9" ht="30.75" customHeight="1">
+      <c r="G20" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="H20" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="I20" s="7" t="s">
+        <v>217</v>
+      </c>
+      <c r="J20" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="K20" s="7" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="21" spans="1:14" ht="30.75" customHeight="1">
       <c r="A21" s="2" t="s">
-        <v>198</v>
-      </c>
-      <c r="B21" s="2" t="s">
+        <v>181</v>
+      </c>
+      <c r="C21" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="D21" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="E21" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="F21" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="G21" s="4" t="s">
+        <v>113</v>
+      </c>
+      <c r="H21" s="4" t="s">
+        <v>226</v>
+      </c>
+      <c r="I21" s="8" t="s">
+        <v>225</v>
+      </c>
+      <c r="J21" s="4" t="s">
+        <v>226</v>
+      </c>
+      <c r="K21" s="8" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="22" spans="1:14" ht="46.5" customHeight="1">
+      <c r="A22" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="B22" s="6"/>
+      <c r="C22" s="5" t="s">
+        <v>103</v>
+      </c>
+      <c r="D22" s="4" t="s">
+        <v>105</v>
+      </c>
+      <c r="E22" s="5" t="s">
+        <v>106</v>
+      </c>
+      <c r="F22" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="G22" s="4" t="s">
+        <v>227</v>
+      </c>
+      <c r="H22" s="4" t="s">
+        <v>226</v>
+      </c>
+      <c r="I22" s="9" t="s">
+        <v>228</v>
+      </c>
+      <c r="J22" s="4" t="s">
+        <v>226</v>
+      </c>
+      <c r="K22" s="9" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="23" spans="1:14" ht="30.75" customHeight="1">
+      <c r="A23" s="2" t="s">
+        <v>183</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="C23" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="D23" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="E23" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="F23" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="G23" s="5" t="s">
+        <v>252</v>
+      </c>
+      <c r="H23" s="4" t="s">
+        <v>224</v>
+      </c>
+      <c r="I23" s="8" t="s">
+        <v>225</v>
+      </c>
+      <c r="J23" s="4" t="s">
+        <v>224</v>
+      </c>
+      <c r="K23" s="8" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="24" spans="1:14" ht="30.75" customHeight="1">
+      <c r="A24" s="2" t="s">
+        <v>184</v>
+      </c>
+      <c r="C24" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="D24" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="E24" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="F24" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="G24" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="H24" s="4" t="s">
+        <v>224</v>
+      </c>
+      <c r="I24" s="8" t="s">
+        <v>225</v>
+      </c>
+      <c r="J24" s="4" t="s">
+        <v>224</v>
+      </c>
+      <c r="K24" s="8" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="25" spans="1:14" ht="30.75" customHeight="1">
+      <c r="A25" s="2" t="s">
+        <v>185</v>
+      </c>
+      <c r="C25" s="5" t="s">
+        <v>90</v>
+      </c>
+      <c r="D25" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="E25" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="F25" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="G25" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="H25" s="4" t="s">
+        <v>224</v>
+      </c>
+      <c r="I25" s="8" t="s">
+        <v>225</v>
+      </c>
+      <c r="J25" s="4" t="s">
+        <v>224</v>
+      </c>
+      <c r="K25" s="8" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="26" spans="1:14" ht="30.75" customHeight="1">
+      <c r="A26" s="2" t="s">
+        <v>186</v>
+      </c>
+      <c r="C26" s="5" t="s">
+        <v>91</v>
+      </c>
+      <c r="D26" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="E26" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="F26" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="G26" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="H26" s="4" t="s">
+        <v>226</v>
+      </c>
+      <c r="I26" s="8" t="s">
+        <v>225</v>
+      </c>
+      <c r="J26" s="4" t="s">
+        <v>226</v>
+      </c>
+      <c r="K26" s="8" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="27" spans="1:14" ht="30.75" customHeight="1">
+      <c r="A27" s="2" t="s">
+        <v>187</v>
+      </c>
+      <c r="C27" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="D27" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="E27" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="F27" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="G27" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="H27" s="4" t="s">
+        <v>226</v>
+      </c>
+      <c r="I27" s="8" t="s">
+        <v>225</v>
+      </c>
+      <c r="J27" s="4" t="s">
+        <v>226</v>
+      </c>
+      <c r="K27" s="8" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="28" spans="1:14" ht="47.25" customHeight="1">
+      <c r="A28" s="2" t="s">
+        <v>188</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="C28" s="4" t="s">
+        <v>231</v>
+      </c>
+      <c r="D28" s="4" t="s">
+        <v>232</v>
+      </c>
+      <c r="E28" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="F28" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="G28" s="5" t="s">
+        <v>253</v>
+      </c>
+      <c r="H28" s="5" t="s">
+        <v>229</v>
+      </c>
+      <c r="I28" s="7" t="s">
+        <v>217</v>
+      </c>
+      <c r="J28" s="5" t="s">
+        <v>229</v>
+      </c>
+      <c r="K28" s="7" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="29" spans="1:14" ht="47.25" customHeight="1">
+      <c r="A29" s="2" t="s">
+        <v>189</v>
+      </c>
+      <c r="C29" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="D29" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="E29" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="F29" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="G29" s="5" t="s">
+        <v>253</v>
+      </c>
+      <c r="H29" s="5" t="s">
+        <v>229</v>
+      </c>
+      <c r="I29" s="9" t="s">
+        <v>228</v>
+      </c>
+      <c r="J29" s="5" t="s">
+        <v>229</v>
+      </c>
+      <c r="K29" s="9" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="30" spans="1:14" ht="47.25" customHeight="1">
+      <c r="A30" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="C30" s="5" t="s">
+        <v>88</v>
+      </c>
+      <c r="D30" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="E30" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="F30" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="G30" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="H30" s="5" t="s">
+        <v>229</v>
+      </c>
+      <c r="I30" s="9" t="s">
+        <v>228</v>
+      </c>
+      <c r="J30" s="5" t="s">
+        <v>229</v>
+      </c>
+      <c r="K30" s="9" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="31" spans="1:14" ht="47.25" customHeight="1">
+      <c r="A31" s="2" t="s">
+        <v>191</v>
+      </c>
+      <c r="C31" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="D31" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="E31" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="F31" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="G31" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="H31" s="5" t="s">
+        <v>229</v>
+      </c>
+      <c r="I31" s="9" t="s">
+        <v>228</v>
+      </c>
+      <c r="J31" s="5" t="s">
+        <v>229</v>
+      </c>
+      <c r="K31" s="9" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="32" spans="1:14" ht="47.25" customHeight="1">
+      <c r="A32" s="2" t="s">
+        <v>192</v>
+      </c>
+      <c r="C32" s="5" t="s">
+        <v>93</v>
+      </c>
+      <c r="D32" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="E32" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="F32" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="G32" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="H32" s="5" t="s">
+        <v>229</v>
+      </c>
+      <c r="I32" s="9" t="s">
+        <v>228</v>
+      </c>
+      <c r="J32" s="5" t="s">
+        <v>229</v>
+      </c>
+      <c r="K32" s="9" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="33" spans="1:11" ht="47.25" customHeight="1">
+      <c r="A33" s="2" t="s">
+        <v>193</v>
+      </c>
+      <c r="C33" s="5" t="s">
+        <v>94</v>
+      </c>
+      <c r="D33" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="E33" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="F33" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="G33" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="H33" s="5" t="s">
+        <v>229</v>
+      </c>
+      <c r="I33" s="9" t="s">
+        <v>228</v>
+      </c>
+      <c r="J33" s="5" t="s">
+        <v>229</v>
+      </c>
+      <c r="K33" s="9" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="34" spans="1:11" ht="47.25" customHeight="1">
+      <c r="A34" s="2" t="s">
+        <v>219</v>
+      </c>
+      <c r="C34" s="5" t="s">
         <v>95</v>
       </c>
-      <c r="C21" s="4" t="s">
-        <v>76</v>
-      </c>
-      <c r="D21" s="4" t="s">
-        <v>77</v>
-      </c>
-      <c r="E21" s="5" t="s">
-        <v>73</v>
-      </c>
-      <c r="F21" s="5" t="s">
-        <v>68</v>
-      </c>
-      <c r="G21" s="4" t="s">
+      <c r="D34" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="E34" s="5" t="s">
         <v>79</v>
       </c>
-      <c r="H21" s="4" t="s">
-        <v>242</v>
-      </c>
-      <c r="I21" s="11" t="s">
-        <v>243</v>
-      </c>
-    </row>
-    <row r="22" spans="1:9" ht="30.75" customHeight="1">
-      <c r="A22" s="2" t="s">
-        <v>199</v>
-      </c>
-      <c r="C22" s="5" t="s">
-        <v>94</v>
-      </c>
-      <c r="D22" s="4" t="s">
-        <v>93</v>
-      </c>
-      <c r="E22" s="5" t="s">
-        <v>73</v>
-      </c>
-      <c r="F22" s="5" t="s">
-        <v>68</v>
-      </c>
-      <c r="G22" s="4" t="s">
-        <v>81</v>
-      </c>
-      <c r="H22" s="4" t="s">
-        <v>242</v>
-      </c>
-      <c r="I22" s="11" t="s">
-        <v>243</v>
-      </c>
-    </row>
-    <row r="23" spans="1:9" ht="30.75" customHeight="1">
-      <c r="A23" s="2" t="s">
-        <v>200</v>
-      </c>
-      <c r="C23" s="5" t="s">
-        <v>99</v>
-      </c>
-      <c r="D23" s="4" t="s">
-        <v>91</v>
-      </c>
-      <c r="E23" s="5" t="s">
-        <v>73</v>
-      </c>
-      <c r="F23" s="5" t="s">
-        <v>68</v>
-      </c>
-      <c r="G23" s="4" t="s">
-        <v>81</v>
-      </c>
-      <c r="H23" s="4" t="s">
-        <v>242</v>
-      </c>
-      <c r="I23" s="11" t="s">
-        <v>243</v>
-      </c>
-    </row>
-    <row r="24" spans="1:9" ht="30.75" customHeight="1">
-      <c r="A24" s="2" t="s">
-        <v>201</v>
-      </c>
-      <c r="C24" s="5" t="s">
-        <v>100</v>
-      </c>
-      <c r="D24" s="4" t="s">
-        <v>92</v>
-      </c>
-      <c r="E24" s="5" t="s">
-        <v>73</v>
-      </c>
-      <c r="F24" s="5" t="s">
-        <v>68</v>
-      </c>
-      <c r="G24" s="4" t="s">
-        <v>81</v>
-      </c>
-      <c r="H24" s="4" t="s">
-        <v>244</v>
-      </c>
-      <c r="I24" s="11" t="s">
-        <v>243</v>
-      </c>
-    </row>
-    <row r="25" spans="1:9" ht="30.75" customHeight="1">
-      <c r="A25" s="2" t="s">
-        <v>202</v>
-      </c>
-      <c r="C25" s="5" t="s">
-        <v>101</v>
-      </c>
-      <c r="D25" s="4" t="s">
+      <c r="F34" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="G34" s="4" t="s">
         <v>80</v>
       </c>
-      <c r="E25" s="5" t="s">
-        <v>73</v>
-      </c>
-      <c r="F25" s="5" t="s">
-        <v>68</v>
-      </c>
-      <c r="G25" s="4" t="s">
-        <v>81</v>
-      </c>
-      <c r="H25" s="4" t="s">
-        <v>244</v>
-      </c>
-      <c r="I25" s="11" t="s">
-        <v>243</v>
-      </c>
-    </row>
-    <row r="26" spans="1:9" ht="47.25" customHeight="1">
-      <c r="A26" s="2" t="s">
-        <v>203</v>
-      </c>
-      <c r="B26" s="2" t="s">
-        <v>96</v>
-      </c>
-      <c r="C26" s="4" t="s">
-        <v>249</v>
-      </c>
-      <c r="D26" s="4" t="s">
-        <v>250</v>
-      </c>
-      <c r="E26" s="5" t="s">
-        <v>84</v>
-      </c>
-      <c r="F26" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="G26" s="4" t="s">
-        <v>85</v>
-      </c>
-      <c r="H26" s="5" t="s">
-        <v>247</v>
-      </c>
-      <c r="I26" s="9" t="s">
-        <v>234</v>
-      </c>
-    </row>
-    <row r="27" spans="1:9" ht="47.25" customHeight="1">
-      <c r="A27" s="2" t="s">
-        <v>204</v>
-      </c>
-      <c r="C27" s="4" t="s">
-        <v>82</v>
-      </c>
-      <c r="D27" s="4" t="s">
-        <v>83</v>
-      </c>
-      <c r="E27" s="5" t="s">
-        <v>84</v>
-      </c>
-      <c r="F27" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="G27" s="4" t="s">
-        <v>85</v>
-      </c>
-      <c r="H27" s="5" t="s">
-        <v>247</v>
-      </c>
-      <c r="I27" s="12" t="s">
-        <v>246</v>
-      </c>
-    </row>
-    <row r="28" spans="1:9" ht="47.25" customHeight="1">
-      <c r="A28" s="2" t="s">
-        <v>205</v>
-      </c>
-      <c r="C28" s="5" t="s">
-        <v>97</v>
-      </c>
-      <c r="D28" s="4" t="s">
-        <v>98</v>
-      </c>
-      <c r="E28" s="5" t="s">
-        <v>84</v>
-      </c>
-      <c r="F28" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="G28" s="4" t="s">
-        <v>89</v>
-      </c>
-      <c r="H28" s="5" t="s">
-        <v>247</v>
-      </c>
-      <c r="I28" s="12" t="s">
-        <v>246</v>
-      </c>
-    </row>
-    <row r="29" spans="1:9" ht="47.25" customHeight="1">
-      <c r="A29" s="2" t="s">
-        <v>206</v>
-      </c>
-      <c r="C29" s="4" t="s">
-        <v>86</v>
-      </c>
-      <c r="D29" s="4" t="s">
-        <v>87</v>
-      </c>
-      <c r="E29" s="5" t="s">
-        <v>88</v>
-      </c>
-      <c r="F29" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="G29" s="4" t="s">
-        <v>89</v>
-      </c>
-      <c r="H29" s="5" t="s">
-        <v>247</v>
-      </c>
-      <c r="I29" s="12" t="s">
-        <v>246</v>
-      </c>
-    </row>
-    <row r="30" spans="1:9" ht="47.25" customHeight="1">
-      <c r="A30" s="2" t="s">
-        <v>207</v>
-      </c>
-      <c r="C30" s="5" t="s">
-        <v>102</v>
-      </c>
-      <c r="D30" s="4" t="s">
-        <v>106</v>
-      </c>
-      <c r="E30" s="5" t="s">
-        <v>88</v>
-      </c>
-      <c r="F30" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="G30" s="4" t="s">
-        <v>89</v>
-      </c>
-      <c r="H30" s="5" t="s">
-        <v>247</v>
-      </c>
-      <c r="I30" s="12" t="s">
-        <v>246</v>
-      </c>
-    </row>
-    <row r="31" spans="1:9" ht="47.25" customHeight="1">
-      <c r="A31" s="2" t="s">
-        <v>208</v>
-      </c>
-      <c r="C31" s="5" t="s">
-        <v>103</v>
-      </c>
-      <c r="D31" s="4" t="s">
-        <v>105</v>
-      </c>
-      <c r="E31" s="5" t="s">
-        <v>88</v>
-      </c>
-      <c r="F31" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="G31" s="4" t="s">
-        <v>89</v>
-      </c>
-      <c r="H31" s="5" t="s">
-        <v>247</v>
-      </c>
-      <c r="I31" s="12" t="s">
-        <v>246</v>
-      </c>
-    </row>
-    <row r="32" spans="1:9" ht="47.25" customHeight="1">
-      <c r="A32" s="2" t="s">
-        <v>209</v>
-      </c>
-      <c r="C32" s="5" t="s">
-        <v>104</v>
-      </c>
-      <c r="D32" s="4" t="s">
-        <v>87</v>
-      </c>
-      <c r="E32" s="5" t="s">
-        <v>88</v>
-      </c>
-      <c r="F32" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="G32" s="4" t="s">
-        <v>89</v>
-      </c>
-      <c r="H32" s="5" t="s">
-        <v>247</v>
-      </c>
-      <c r="I32" s="12" t="s">
-        <v>246</v>
-      </c>
-    </row>
-    <row r="33" spans="1:9" ht="30.75" customHeight="1">
-      <c r="A33" s="2" t="s">
-        <v>210</v>
-      </c>
-      <c r="B33" s="2" t="s">
-        <v>119</v>
-      </c>
-      <c r="C33" s="4" t="s">
-        <v>120</v>
-      </c>
-      <c r="D33" s="4" t="s">
-        <v>121</v>
-      </c>
-      <c r="E33" s="4" t="s">
-        <v>122</v>
-      </c>
-      <c r="G33" s="5" t="s">
-        <v>123</v>
-      </c>
-      <c r="H33" s="4" t="s">
-        <v>248</v>
-      </c>
-      <c r="I33" s="9" t="s">
-        <v>234</v>
-      </c>
-    </row>
-    <row r="34" spans="1:9" ht="45" customHeight="1">
-      <c r="A34" s="2" t="s">
-        <v>236</v>
-      </c>
-      <c r="B34" s="6" t="s">
-        <v>147</v>
-      </c>
-      <c r="C34" s="7" t="s">
-        <v>151</v>
-      </c>
-      <c r="D34" s="8"/>
-    </row>
-    <row r="36" spans="1:9" ht="30.75" customHeight="1">
-      <c r="B36" s="2">
-        <v>31743</v>
-      </c>
-      <c r="C36" s="2">
-        <v>131870</v>
-      </c>
-    </row>
-    <row r="37" spans="1:9" ht="30.75" customHeight="1">
-      <c r="C37" s="2">
-        <v>131871</v>
-      </c>
-    </row>
-    <row r="38" spans="1:9" ht="30.75" customHeight="1">
-      <c r="C38" s="2">
-        <v>131873</v>
-      </c>
-    </row>
-    <row r="39" spans="1:9" ht="30.75" customHeight="1">
-      <c r="C39" s="2"/>
-    </row>
-    <row r="40" spans="1:9" ht="30.75" customHeight="1">
-      <c r="B40" s="2">
-        <v>35613</v>
-      </c>
-      <c r="C40" s="2">
-        <v>131872</v>
-      </c>
+      <c r="H34" s="5" t="s">
+        <v>229</v>
+      </c>
+      <c r="I34" s="9" t="s">
+        <v>228</v>
+      </c>
+      <c r="J34" s="5" t="s">
+        <v>229</v>
+      </c>
+      <c r="K34" s="9" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="35" spans="1:11" ht="30.75" customHeight="1">
+      <c r="A35" s="2" t="s">
+        <v>268</v>
+      </c>
+      <c r="B35" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="C35" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="D35" s="4" t="s">
+        <v>110</v>
+      </c>
+      <c r="E35" s="4" t="s">
+        <v>111</v>
+      </c>
+      <c r="G35" s="5" t="s">
+        <v>112</v>
+      </c>
+      <c r="H35" s="4" t="s">
+        <v>230</v>
+      </c>
+      <c r="I35" s="7" t="s">
+        <v>217</v>
+      </c>
+      <c r="J35" s="4" t="s">
+        <v>230</v>
+      </c>
+      <c r="K35" s="7" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="36" spans="1:11" ht="45" customHeight="1">
+      <c r="A36" s="2" t="s">
+        <v>269</v>
+      </c>
+      <c r="B36" s="6" t="s">
+        <v>132</v>
+      </c>
+      <c r="C36" s="10" t="s">
+        <v>136</v>
+      </c>
+      <c r="D36" s="11"/>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="C34:D34"/>
+    <mergeCell ref="C36:D36"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2664,26 +2985,30 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{76EA9C7D-F9B9-4927-9349-23AE4A85C0E3}">
-  <dimension ref="A1:L21"/>
+  <dimension ref="A1:M22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="M11" sqref="M11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="30.75" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="10.140625" style="2" customWidth="1"/>
-    <col min="2" max="2" width="21.28515625" style="2" customWidth="1"/>
-    <col min="3" max="3" width="47.42578125" style="4" customWidth="1"/>
-    <col min="4" max="4" width="46.140625" style="4" customWidth="1"/>
-    <col min="5" max="5" width="47.85546875" style="4" customWidth="1"/>
+    <col min="2" max="2" width="11.42578125" style="2" customWidth="1"/>
+    <col min="3" max="3" width="42" style="4" customWidth="1"/>
+    <col min="4" max="4" width="42.7109375" style="4" customWidth="1"/>
+    <col min="5" max="5" width="46.5703125" style="4" customWidth="1"/>
     <col min="6" max="6" width="20.140625" style="4" customWidth="1"/>
     <col min="7" max="7" width="32.28515625" style="4" customWidth="1"/>
-    <col min="8" max="9" width="16.85546875" style="4" customWidth="1"/>
-    <col min="10" max="16384" width="9.140625" style="4"/>
+    <col min="8" max="8" width="29.5703125" style="4" customWidth="1"/>
+    <col min="9" max="9" width="9.42578125" style="4" customWidth="1"/>
+    <col min="10" max="10" width="30.85546875" style="4" customWidth="1"/>
+    <col min="11" max="11" width="9.42578125" style="4" customWidth="1"/>
+    <col min="12" max="13" width="11.140625" style="4" customWidth="1"/>
+    <col min="14" max="16384" width="9.140625" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="19.5" customHeight="1">
+    <row r="1" spans="1:13" ht="19.5" customHeight="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2706,30 +3031,36 @@
         <v>6</v>
       </c>
       <c r="H1" s="3" t="s">
-        <v>14</v>
+        <v>248</v>
       </c>
       <c r="I1" s="3" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="2" spans="1:12" ht="44.25" customHeight="1">
+      <c r="J1" s="3" t="s">
+        <v>249</v>
+      </c>
+      <c r="K1" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" ht="30.75" customHeight="1">
       <c r="A2" s="2" t="s">
-        <v>211</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>118</v>
+        <v>194</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>235</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>126</v>
+        <v>115</v>
       </c>
       <c r="D2" s="5" t="s">
         <v>8</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>130</v>
+        <v>117</v>
       </c>
       <c r="F2" s="5" t="s">
-        <v>149</v>
+        <v>134</v>
       </c>
       <c r="G2" s="4" t="s">
         <v>24</v>
@@ -2737,31 +3068,33 @@
       <c r="H2" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="I2" s="9" t="s">
-        <v>234</v>
-      </c>
-      <c r="K2" s="2">
-        <v>31743</v>
-      </c>
-      <c r="L2" s="2">
-        <v>131870</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12" ht="30.75" customHeight="1">
+      <c r="I2" s="7" t="s">
+        <v>217</v>
+      </c>
+      <c r="J2" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="K2" s="7" t="s">
+        <v>217</v>
+      </c>
+      <c r="L2" s="2"/>
+      <c r="M2" s="2"/>
+    </row>
+    <row r="3" spans="1:13" ht="30.75" customHeight="1">
       <c r="A3" s="2" t="s">
-        <v>212</v>
-      </c>
-      <c r="C3" s="4" t="s">
-        <v>127</v>
+        <v>195</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>241</v>
       </c>
       <c r="D3" s="4" t="s">
         <v>9</v>
       </c>
       <c r="E3" s="5" t="s">
-        <v>131</v>
+        <v>118</v>
       </c>
       <c r="F3" s="5" t="s">
-        <v>148</v>
+        <v>133</v>
       </c>
       <c r="G3" s="4" t="s">
         <v>24</v>
@@ -2769,26 +3102,30 @@
       <c r="H3" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="I3" s="9" t="s">
-        <v>234</v>
-      </c>
-      <c r="K3" s="2"/>
-      <c r="L3" s="2">
-        <v>131871</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" ht="30.75" customHeight="1">
+      <c r="I3" s="7" t="s">
+        <v>217</v>
+      </c>
+      <c r="J3" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="K3" s="7" t="s">
+        <v>217</v>
+      </c>
+      <c r="L3" s="2"/>
+      <c r="M3" s="2"/>
+    </row>
+    <row r="4" spans="1:13" ht="30.75" customHeight="1">
       <c r="A4" s="2" t="s">
-        <v>213</v>
-      </c>
-      <c r="C4" s="4" t="s">
-        <v>128</v>
+        <v>196</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>239</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>150</v>
+        <v>135</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>132</v>
+        <v>119</v>
       </c>
       <c r="F4" s="5" t="s">
         <v>18</v>
@@ -2799,20 +3136,24 @@
       <c r="H4" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="I4" s="9" t="s">
-        <v>234</v>
-      </c>
-      <c r="K4" s="2"/>
-      <c r="L4" s="2">
-        <v>131873</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" ht="32.25" customHeight="1">
+      <c r="I4" s="7" t="s">
+        <v>217</v>
+      </c>
+      <c r="J4" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="K4" s="7" t="s">
+        <v>217</v>
+      </c>
+      <c r="L4" s="2"/>
+      <c r="M4" s="2"/>
+    </row>
+    <row r="5" spans="1:13" ht="32.25" customHeight="1">
       <c r="A5" s="2" t="s">
-        <v>214</v>
+        <v>197</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>129</v>
+        <v>116</v>
       </c>
       <c r="D5" s="4" t="s">
         <v>10</v>
@@ -2827,17 +3168,23 @@
         <v>26</v>
       </c>
       <c r="H5" s="5" t="s">
-        <v>251</v>
-      </c>
-      <c r="I5" s="9" t="s">
-        <v>234</v>
-      </c>
-      <c r="K5" s="2"/>
+        <v>233</v>
+      </c>
+      <c r="I5" s="7" t="s">
+        <v>217</v>
+      </c>
+      <c r="J5" s="5" t="s">
+        <v>233</v>
+      </c>
+      <c r="K5" s="7" t="s">
+        <v>217</v>
+      </c>
       <c r="L5" s="2"/>
-    </row>
-    <row r="6" spans="1:12" ht="32.25" customHeight="1">
+      <c r="M5" s="2"/>
+    </row>
+    <row r="6" spans="1:13" ht="32.25" customHeight="1">
       <c r="A6" s="2" t="s">
-        <v>215</v>
+        <v>198</v>
       </c>
       <c r="C6" s="4" t="s">
         <v>30</v>
@@ -2857,19 +3204,21 @@
       <c r="H6" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="I6" s="9" t="s">
-        <v>234</v>
-      </c>
-      <c r="K6" s="2">
-        <v>35613</v>
-      </c>
-      <c r="L6" s="2">
-        <v>131872</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12" ht="32.25" customHeight="1">
+      <c r="I6" s="7" t="s">
+        <v>217</v>
+      </c>
+      <c r="J6" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="K6" s="7" t="s">
+        <v>217</v>
+      </c>
+      <c r="L6" s="2"/>
+      <c r="M6" s="2"/>
+    </row>
+    <row r="7" spans="1:13" ht="32.25" customHeight="1">
       <c r="A7" s="2" t="s">
-        <v>216</v>
+        <v>199</v>
       </c>
       <c r="C7" s="4" t="s">
         <v>31</v>
@@ -2889,309 +3238,532 @@
       <c r="H7" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="I7" s="9" t="s">
-        <v>234</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12" ht="32.25" customHeight="1">
+      <c r="I7" s="7" t="s">
+        <v>217</v>
+      </c>
+      <c r="J7" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="K7" s="7" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" ht="32.25" customHeight="1">
       <c r="A8" s="2" t="s">
-        <v>217</v>
+        <v>200</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>141</v>
+        <v>126</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>142</v>
+        <v>127</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>135</v>
+        <v>121</v>
       </c>
       <c r="E8" s="5" t="s">
-        <v>73</v>
+        <v>66</v>
       </c>
       <c r="F8" s="5" t="s">
-        <v>68</v>
+        <v>61</v>
       </c>
       <c r="G8" s="5" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12" ht="32.25" customHeight="1">
+        <v>122</v>
+      </c>
+      <c r="H8" s="4" t="s">
+        <v>224</v>
+      </c>
+      <c r="I8" s="8" t="s">
+        <v>225</v>
+      </c>
+      <c r="J8" s="4" t="s">
+        <v>224</v>
+      </c>
+      <c r="K8" s="8" t="s">
+        <v>225</v>
+      </c>
+      <c r="L8" s="6" t="s">
+        <v>270</v>
+      </c>
+      <c r="M8" s="6" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" ht="32.25" customHeight="1">
       <c r="A9" s="2" t="s">
-        <v>218</v>
+        <v>201</v>
       </c>
       <c r="B9" s="6"/>
       <c r="C9" s="5" t="s">
-        <v>143</v>
+        <v>128</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>144</v>
+        <v>129</v>
       </c>
       <c r="E9" s="5" t="s">
-        <v>153</v>
+        <v>138</v>
       </c>
       <c r="F9" s="5" t="s">
-        <v>152</v>
+        <v>137</v>
       </c>
       <c r="G9" s="5" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="10" spans="1:12" ht="32.25" customHeight="1">
+        <v>130</v>
+      </c>
+      <c r="H9" s="4" t="s">
+        <v>224</v>
+      </c>
+      <c r="I9" s="8" t="s">
+        <v>225</v>
+      </c>
+      <c r="J9" s="5" t="s">
+        <v>276</v>
+      </c>
+      <c r="K9" s="7" t="s">
+        <v>217</v>
+      </c>
+      <c r="L9" s="2"/>
+      <c r="M9" s="6" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" ht="32.25" customHeight="1">
       <c r="A10" s="2" t="s">
-        <v>219</v>
+        <v>202</v>
       </c>
       <c r="B10" s="6"/>
       <c r="C10" s="5" t="s">
-        <v>146</v>
+        <v>131</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>154</v>
+        <v>139</v>
       </c>
       <c r="E10" s="5" t="s">
-        <v>155</v>
+        <v>140</v>
       </c>
       <c r="F10" s="5" t="s">
+        <v>141</v>
+      </c>
+      <c r="G10" s="5" t="s">
+        <v>142</v>
+      </c>
+      <c r="H10" s="4" t="s">
+        <v>224</v>
+      </c>
+      <c r="I10" s="8" t="s">
+        <v>225</v>
+      </c>
+      <c r="J10" s="5" t="s">
+        <v>276</v>
+      </c>
+      <c r="K10" s="7" t="s">
+        <v>217</v>
+      </c>
+      <c r="L10" s="2"/>
+      <c r="M10" s="6" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" ht="32.25" customHeight="1">
+      <c r="A11" s="2" t="s">
+        <v>203</v>
+      </c>
+      <c r="B11" s="6" t="s">
+        <v>236</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>240</v>
+      </c>
+      <c r="D11" s="4" t="s">
+        <v>158</v>
+      </c>
+      <c r="E11" s="5" t="s">
         <v>156</v>
       </c>
-      <c r="G10" s="5" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="11" spans="1:12" ht="32.25" customHeight="1">
-      <c r="A11" s="2" t="s">
-        <v>220</v>
-      </c>
-      <c r="B11" s="6" t="s">
-        <v>158</v>
-      </c>
-      <c r="C11" s="4" t="s">
-        <v>69</v>
-      </c>
-      <c r="D11" s="4" t="s">
-        <v>174</v>
-      </c>
-      <c r="E11" s="5" t="s">
-        <v>172</v>
-      </c>
       <c r="F11" s="5" t="s">
-        <v>167</v>
+        <v>151</v>
       </c>
       <c r="G11" s="5" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="12" spans="1:12" ht="32.25" customHeight="1">
+        <v>120</v>
+      </c>
+      <c r="H11" s="5" t="s">
+        <v>120</v>
+      </c>
+      <c r="I11" s="7" t="s">
+        <v>217</v>
+      </c>
+      <c r="J11" s="5" t="s">
+        <v>120</v>
+      </c>
+      <c r="K11" s="7" t="s">
+        <v>217</v>
+      </c>
+      <c r="L11" s="2"/>
+      <c r="M11" s="2"/>
+    </row>
+    <row r="12" spans="1:13" ht="32.25" customHeight="1">
       <c r="A12" s="2" t="s">
-        <v>221</v>
+        <v>204</v>
       </c>
       <c r="B12" s="6"/>
       <c r="C12" s="5" t="s">
-        <v>159</v>
+        <v>143</v>
       </c>
       <c r="D12" s="5" t="s">
-        <v>160</v>
+        <v>144</v>
       </c>
       <c r="E12" s="5" t="s">
-        <v>162</v>
+        <v>146</v>
       </c>
       <c r="F12" s="5" t="s">
-        <v>167</v>
+        <v>151</v>
       </c>
       <c r="G12" s="5" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="13" spans="1:12" ht="32.25" customHeight="1">
+        <v>145</v>
+      </c>
+      <c r="H12" s="5" t="s">
+        <v>145</v>
+      </c>
+      <c r="I12" s="7" t="s">
+        <v>217</v>
+      </c>
+      <c r="J12" s="5" t="s">
+        <v>145</v>
+      </c>
+      <c r="K12" s="7" t="s">
+        <v>217</v>
+      </c>
+      <c r="L12" s="6" t="s">
+        <v>274</v>
+      </c>
+      <c r="M12" s="6" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" ht="32.25" customHeight="1">
       <c r="A13" s="2" t="s">
-        <v>222</v>
+        <v>205</v>
       </c>
       <c r="B13" s="6"/>
       <c r="C13" s="5" t="s">
-        <v>163</v>
+        <v>147</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>164</v>
+        <v>148</v>
       </c>
       <c r="E13" s="5" t="s">
-        <v>169</v>
+        <v>153</v>
       </c>
       <c r="F13" s="5" t="s">
-        <v>168</v>
+        <v>152</v>
       </c>
       <c r="G13" s="5" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="14" spans="1:12" ht="32.25" customHeight="1">
+        <v>123</v>
+      </c>
+      <c r="H13" s="5" t="s">
+        <v>242</v>
+      </c>
+      <c r="I13" s="9" t="s">
+        <v>228</v>
+      </c>
+      <c r="J13" s="5" t="s">
+        <v>242</v>
+      </c>
+      <c r="K13" s="9" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" ht="32.25" customHeight="1">
       <c r="A14" s="2" t="s">
-        <v>223</v>
+        <v>206</v>
       </c>
       <c r="B14" s="6"/>
       <c r="C14" s="5" t="s">
-        <v>165</v>
+        <v>149</v>
       </c>
       <c r="D14" s="4" t="s">
-        <v>166</v>
+        <v>150</v>
       </c>
       <c r="E14" s="5" t="s">
-        <v>170</v>
+        <v>154</v>
       </c>
       <c r="F14" s="5" t="s">
-        <v>167</v>
+        <v>151</v>
       </c>
       <c r="G14" s="5" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="15" spans="1:12" ht="32.25" customHeight="1">
+        <v>123</v>
+      </c>
+      <c r="H14" s="5" t="s">
+        <v>120</v>
+      </c>
+      <c r="I14" s="8" t="s">
+        <v>225</v>
+      </c>
+      <c r="J14" s="5" t="s">
+        <v>277</v>
+      </c>
+      <c r="K14" s="7" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" ht="32.25" customHeight="1">
       <c r="A15" s="2" t="s">
-        <v>224</v>
+        <v>207</v>
       </c>
       <c r="B15" s="6"/>
       <c r="C15" s="5" t="s">
-        <v>134</v>
+        <v>238</v>
       </c>
       <c r="D15" s="5" t="s">
-        <v>173</v>
+        <v>157</v>
       </c>
       <c r="E15" s="5" t="s">
-        <v>171</v>
+        <v>155</v>
       </c>
       <c r="F15" s="5" t="s">
-        <v>167</v>
+        <v>151</v>
       </c>
       <c r="G15" s="5" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="16" spans="1:12" ht="32.25" customHeight="1">
+        <v>123</v>
+      </c>
+      <c r="H15" s="5" t="s">
+        <v>243</v>
+      </c>
+      <c r="I15" s="7" t="s">
+        <v>217</v>
+      </c>
+      <c r="J15" s="5" t="s">
+        <v>243</v>
+      </c>
+      <c r="K15" s="7" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" ht="32.25" customHeight="1">
       <c r="A16" s="2" t="s">
+        <v>208</v>
+      </c>
+      <c r="B16" s="6" t="s">
+        <v>125</v>
+      </c>
+      <c r="C16" s="4" t="s">
+        <v>124</v>
+      </c>
+      <c r="D16" s="4" t="s">
+        <v>121</v>
+      </c>
+      <c r="E16" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="F16" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="G16" s="4" t="s">
+        <v>214</v>
+      </c>
+      <c r="H16" s="4" t="s">
+        <v>226</v>
+      </c>
+      <c r="I16" s="8" t="s">
         <v>225</v>
       </c>
-      <c r="B16" s="6" t="s">
-        <v>139</v>
-      </c>
-      <c r="C16" s="4" t="s">
-        <v>138</v>
-      </c>
-      <c r="D16" s="4" t="s">
-        <v>135</v>
-      </c>
-      <c r="E16" s="5" t="s">
-        <v>73</v>
-      </c>
-      <c r="F16" s="5" t="s">
-        <v>68</v>
-      </c>
-      <c r="G16" s="4" t="s">
-        <v>231</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" ht="32.25" customHeight="1">
+      <c r="J16" s="4" t="s">
+        <v>226</v>
+      </c>
+      <c r="K16" s="8" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" ht="32.25" customHeight="1">
       <c r="A17" s="2" t="s">
-        <v>226</v>
+        <v>209</v>
       </c>
       <c r="B17" s="6"/>
       <c r="C17" s="5" t="s">
-        <v>177</v>
+        <v>161</v>
       </c>
       <c r="D17" s="4" t="s">
-        <v>175</v>
+        <v>245</v>
       </c>
       <c r="E17" s="5" t="s">
-        <v>176</v>
+        <v>246</v>
       </c>
       <c r="F17" s="5" t="s">
-        <v>156</v>
+        <v>137</v>
       </c>
       <c r="G17" s="4" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" ht="30.75" customHeight="1">
+        <v>114</v>
+      </c>
+      <c r="H17" s="4" t="s">
+        <v>226</v>
+      </c>
+      <c r="I17" s="8" t="s">
+        <v>225</v>
+      </c>
+      <c r="J17" s="4" t="s">
+        <v>226</v>
+      </c>
+      <c r="K17" s="8" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" ht="32.25" customHeight="1">
       <c r="A18" s="2" t="s">
-        <v>227</v>
-      </c>
-      <c r="B18" s="2" t="s">
-        <v>140</v>
-      </c>
-      <c r="C18" s="4" t="s">
-        <v>71</v>
-      </c>
-      <c r="D18" s="5" t="s">
-        <v>72</v>
+        <v>210</v>
+      </c>
+      <c r="B18" s="6"/>
+      <c r="C18" s="5" t="s">
+        <v>244</v>
+      </c>
+      <c r="D18" s="4" t="s">
+        <v>159</v>
       </c>
       <c r="E18" s="5" t="s">
-        <v>73</v>
+        <v>160</v>
       </c>
       <c r="F18" s="5" t="s">
-        <v>68</v>
+        <v>141</v>
       </c>
       <c r="G18" s="4" t="s">
-        <v>232</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" ht="32.25" customHeight="1">
+        <v>114</v>
+      </c>
+      <c r="H18" s="5" t="s">
+        <v>242</v>
+      </c>
+      <c r="I18" s="9" t="s">
+        <v>228</v>
+      </c>
+      <c r="J18" s="5" t="s">
+        <v>242</v>
+      </c>
+      <c r="K18" s="9" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" ht="30.75" customHeight="1">
       <c r="A19" s="2" t="s">
-        <v>228</v>
-      </c>
-      <c r="B19" s="6"/>
-      <c r="C19" s="5" t="s">
-        <v>178</v>
-      </c>
-      <c r="D19" s="4" t="s">
-        <v>175</v>
+        <v>211</v>
+      </c>
+      <c r="B19" s="6" t="s">
+        <v>234</v>
+      </c>
+      <c r="C19" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="D19" s="5" t="s">
+        <v>65</v>
       </c>
       <c r="E19" s="5" t="s">
-        <v>176</v>
+        <v>66</v>
       </c>
       <c r="F19" s="5" t="s">
-        <v>156</v>
+        <v>61</v>
       </c>
       <c r="G19" s="4" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" ht="46.5" customHeight="1">
+        <v>215</v>
+      </c>
+      <c r="H19" s="4" t="s">
+        <v>226</v>
+      </c>
+      <c r="I19" s="8" t="s">
+        <v>225</v>
+      </c>
+      <c r="J19" s="4" t="s">
+        <v>226</v>
+      </c>
+      <c r="K19" s="8" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" ht="32.25" customHeight="1">
       <c r="A20" s="2" t="s">
-        <v>229</v>
+        <v>212</v>
       </c>
       <c r="B20" s="6"/>
       <c r="C20" s="5" t="s">
+        <v>237</v>
+      </c>
+      <c r="D20" s="4" t="s">
+        <v>245</v>
+      </c>
+      <c r="E20" s="5" t="s">
+        <v>246</v>
+      </c>
+      <c r="F20" s="5" t="s">
+        <v>137</v>
+      </c>
+      <c r="G20" s="4" t="s">
         <v>114</v>
       </c>
-      <c r="D20" s="4" t="s">
-        <v>116</v>
-      </c>
-      <c r="E20" s="5" t="s">
-        <v>117</v>
-      </c>
-      <c r="F20" s="5" t="s">
-        <v>68</v>
-      </c>
-      <c r="G20" s="4" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" ht="30.75" customHeight="1">
+      <c r="H20" s="5" t="s">
+        <v>242</v>
+      </c>
+      <c r="I20" s="9" t="s">
+        <v>228</v>
+      </c>
+      <c r="J20" s="5" t="s">
+        <v>242</v>
+      </c>
+      <c r="K20" s="9" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" ht="46.5" customHeight="1">
       <c r="A21" s="2" t="s">
-        <v>230</v>
-      </c>
-      <c r="B21" s="2" t="s">
-        <v>119</v>
-      </c>
-      <c r="C21" s="4" t="s">
-        <v>120</v>
+        <v>213</v>
+      </c>
+      <c r="B21" s="6"/>
+      <c r="C21" s="5" t="s">
+        <v>103</v>
       </c>
       <c r="D21" s="4" t="s">
-        <v>121</v>
-      </c>
-      <c r="E21" s="4" t="s">
-        <v>122</v>
-      </c>
-      <c r="G21" s="5" t="s">
-        <v>123</v>
+        <v>105</v>
+      </c>
+      <c r="E21" s="5" t="s">
+        <v>106</v>
+      </c>
+      <c r="F21" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="G21" s="4" t="s">
+        <v>114</v>
+      </c>
+      <c r="H21" s="4" t="s">
+        <v>226</v>
+      </c>
+      <c r="I21" s="9" t="s">
+        <v>228</v>
+      </c>
+      <c r="J21" s="4" t="s">
+        <v>226</v>
+      </c>
+      <c r="K21" s="9" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" ht="30.75" customHeight="1">
+      <c r="A22" s="2" t="s">
+        <v>247</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="C22" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="D22" s="4" t="s">
+        <v>110</v>
+      </c>
+      <c r="E22" s="4" t="s">
+        <v>111</v>
+      </c>
+      <c r="G22" s="5" t="s">
+        <v>112</v>
+      </c>
+      <c r="H22" s="5" t="s">
+        <v>112</v>
+      </c>
+      <c r="I22" s="7" t="s">
+        <v>217</v>
       </c>
     </row>
   </sheetData>

</xml_diff>